<commit_message>
updated through 2019-04-01 15:00
</commit_message>
<xml_diff>
--- a/librelink/Librelink.xlsx
+++ b/librelink/Librelink.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8bc6084b92ffa451/Sprague 2019/Health 2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="13_ncr:1_{1DF15EB1-8D61-6642-9AC4-0A049F576367}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{55C9846D-999F-2240-A4EF-0F4E8FA43194}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="13_ncr:1_{1DF15EB1-8D61-6642-9AC4-0A049F576367}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{932C1E46-D17F-0F46-A54C-2F381D15E3A1}"/>
   <bookViews>
     <workbookView xWindow="13920" yWindow="1180" windowWidth="17400" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="67">
   <si>
     <t>Meter</t>
   </si>
@@ -226,6 +226,9 @@
   </si>
   <si>
     <t>Burger</t>
+  </si>
+  <si>
+    <t>Whole wheat</t>
   </si>
 </sst>
 </file>
@@ -791,8 +794,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF602BB5-9469-1B45-BB1A-DFBEABAFCD1B}" name="Table1" displayName="Table1" ref="A1:S4083" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:S4083" xr:uid="{A8E95FAB-7D33-F24D-8350-CC174D759A60}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF602BB5-9469-1B45-BB1A-DFBEABAFCD1B}" name="Table1" displayName="Table1" ref="A1:S4131" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:S4131" xr:uid="{A8E95FAB-7D33-F24D-8350-CC174D759A60}"/>
   <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{374D21D6-0283-C44B-8028-4060CB201675}" name="Meter"/>
     <tableColumn id="2" xr3:uid="{48610F22-94E8-1142-AF15-100D6756BE81}" name="Serial Number"/>
@@ -1115,12 +1118,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S4083"/>
+  <dimension ref="A1:S4131"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4001" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A4062" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="C4018" sqref="C4018"/>
+      <selection pane="bottomLeft" activeCell="C4084" sqref="C4084:N4131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -47642,7 +47645,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4081" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="4081" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C4081" s="1">
         <v>43556.275000000001</v>
       </c>
@@ -47653,7 +47656,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4082" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="4082" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C4082" s="1">
         <v>43556.283333333333</v>
       </c>
@@ -47664,7 +47667,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4083" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="4083" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C4083" s="1">
         <v>43556.287499999999</v>
       </c>
@@ -47673,6 +47676,534 @@
       </c>
       <c r="F4083">
         <v>83</v>
+      </c>
+    </row>
+    <row r="4084" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4084" s="1">
+        <v>43556.296527777777</v>
+      </c>
+      <c r="D4084">
+        <v>0</v>
+      </c>
+      <c r="E4084">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4085" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4085" s="1">
+        <v>43556.306250000001</v>
+      </c>
+      <c r="D4085">
+        <v>0</v>
+      </c>
+      <c r="E4085">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4086" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4086" s="1">
+        <v>43556.311805555553</v>
+      </c>
+      <c r="D4086">
+        <v>1</v>
+      </c>
+      <c r="F4086">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4087" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4087" s="1">
+        <v>43556.311805555553</v>
+      </c>
+      <c r="D4087">
+        <v>6</v>
+      </c>
+      <c r="N4087" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4088" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4088" s="1">
+        <v>43556.317361111112</v>
+      </c>
+      <c r="D4088">
+        <v>0</v>
+      </c>
+      <c r="E4088">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4089" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4089" s="1">
+        <v>43556.317361111112</v>
+      </c>
+      <c r="D4089">
+        <v>1</v>
+      </c>
+      <c r="F4089">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4090" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4090" s="1">
+        <v>43556.321527777778</v>
+      </c>
+      <c r="D4090">
+        <v>1</v>
+      </c>
+      <c r="F4090">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4091" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4091" s="1">
+        <v>43556.327777777777</v>
+      </c>
+      <c r="D4091">
+        <v>0</v>
+      </c>
+      <c r="E4091">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4092" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4092" s="1">
+        <v>43556.329861111109</v>
+      </c>
+      <c r="D4092">
+        <v>1</v>
+      </c>
+      <c r="F4092">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4093" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4093" s="1">
+        <v>43556.338194444441</v>
+      </c>
+      <c r="D4093">
+        <v>0</v>
+      </c>
+      <c r="E4093">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4094" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4094" s="1">
+        <v>43556.34375</v>
+      </c>
+      <c r="D4094">
+        <v>1</v>
+      </c>
+      <c r="F4094">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4095" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4095" s="1">
+        <v>43556.348611111112</v>
+      </c>
+      <c r="D4095">
+        <v>0</v>
+      </c>
+      <c r="E4095">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4096" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4096" s="1">
+        <v>43556.350694444445</v>
+      </c>
+      <c r="D4096">
+        <v>1</v>
+      </c>
+      <c r="F4096">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4097" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4097" s="1">
+        <v>43556.359027777777</v>
+      </c>
+      <c r="D4097">
+        <v>1</v>
+      </c>
+      <c r="F4097">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4098" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4098" s="1">
+        <v>43556.359722222223</v>
+      </c>
+      <c r="D4098">
+        <v>0</v>
+      </c>
+      <c r="E4098">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4099" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4099" s="1">
+        <v>43556.370138888888</v>
+      </c>
+      <c r="D4099">
+        <v>0</v>
+      </c>
+      <c r="E4099">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4100" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4100" s="1">
+        <v>43556.376388888886</v>
+      </c>
+      <c r="D4100">
+        <v>1</v>
+      </c>
+      <c r="F4100">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4101" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4101" s="1">
+        <v>43556.380555555559</v>
+      </c>
+      <c r="D4101">
+        <v>0</v>
+      </c>
+      <c r="E4101">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4102" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4102" s="1">
+        <v>43556.390972222223</v>
+      </c>
+      <c r="D4102">
+        <v>0</v>
+      </c>
+      <c r="E4102">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4103" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4103" s="1">
+        <v>43556.398611111108</v>
+      </c>
+      <c r="D4103">
+        <v>1</v>
+      </c>
+      <c r="F4103">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4104" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4104" s="1">
+        <v>43556.401388888888</v>
+      </c>
+      <c r="D4104">
+        <v>0</v>
+      </c>
+      <c r="E4104">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4105" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4105" s="1">
+        <v>43556.412499999999</v>
+      </c>
+      <c r="D4105">
+        <v>0</v>
+      </c>
+      <c r="E4105">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4106" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4106" s="1">
+        <v>43556.418055555558</v>
+      </c>
+      <c r="D4106">
+        <v>1</v>
+      </c>
+      <c r="F4106">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4107" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4107" s="1">
+        <v>43556.42291666667</v>
+      </c>
+      <c r="D4107">
+        <v>0</v>
+      </c>
+      <c r="E4107">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4108" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4108" s="1">
+        <v>43556.433333333334</v>
+      </c>
+      <c r="D4108">
+        <v>0</v>
+      </c>
+      <c r="E4108">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4109" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4109" s="1">
+        <v>43556.443749999999</v>
+      </c>
+      <c r="D4109">
+        <v>0</v>
+      </c>
+      <c r="E4109">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4110" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4110" s="1">
+        <v>43556.45416666667</v>
+      </c>
+      <c r="D4110">
+        <v>0</v>
+      </c>
+      <c r="E4110">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4111" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4111" s="1">
+        <v>43556.464583333334</v>
+      </c>
+      <c r="D4111">
+        <v>0</v>
+      </c>
+      <c r="E4111">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4112" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4112" s="1">
+        <v>43556.474999999999</v>
+      </c>
+      <c r="D4112">
+        <v>0</v>
+      </c>
+      <c r="E4112">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4113" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4113" s="1">
+        <v>43556.48541666667</v>
+      </c>
+      <c r="D4113">
+        <v>0</v>
+      </c>
+      <c r="E4113">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4114" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4114" s="1">
+        <v>43556.495833333334</v>
+      </c>
+      <c r="D4114">
+        <v>0</v>
+      </c>
+      <c r="E4114">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4115" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4115" s="1">
+        <v>43556.506249999999</v>
+      </c>
+      <c r="D4115">
+        <v>0</v>
+      </c>
+      <c r="E4115">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4116" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4116" s="1">
+        <v>43556.51666666667</v>
+      </c>
+      <c r="D4116">
+        <v>0</v>
+      </c>
+      <c r="E4116">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4117" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4117" s="1">
+        <v>43556.527083333334</v>
+      </c>
+      <c r="D4117">
+        <v>0</v>
+      </c>
+      <c r="E4117">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4118" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4118" s="1">
+        <v>43556.538194444445</v>
+      </c>
+      <c r="D4118">
+        <v>0</v>
+      </c>
+      <c r="E4118">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4119" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4119" s="1">
+        <v>43556.541666666664</v>
+      </c>
+      <c r="D4119">
+        <v>1</v>
+      </c>
+      <c r="F4119">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4120" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4120" s="1">
+        <v>43556.548611111109</v>
+      </c>
+      <c r="D4120">
+        <v>0</v>
+      </c>
+      <c r="E4120">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4121" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4121" s="1">
+        <v>43556.559027777781</v>
+      </c>
+      <c r="D4121">
+        <v>0</v>
+      </c>
+      <c r="E4121">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4122" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4122" s="1">
+        <v>43556.570138888892</v>
+      </c>
+      <c r="D4122">
+        <v>0</v>
+      </c>
+      <c r="E4122">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4123" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4123" s="1">
+        <v>43556.574305555558</v>
+      </c>
+      <c r="D4123">
+        <v>1</v>
+      </c>
+      <c r="F4123">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4124" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4124" s="1">
+        <v>43556.580555555556</v>
+      </c>
+      <c r="D4124">
+        <v>0</v>
+      </c>
+      <c r="E4124">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4125" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4125" s="1">
+        <v>43556.59097222222</v>
+      </c>
+      <c r="D4125">
+        <v>0</v>
+      </c>
+      <c r="E4125">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4126" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4126" s="1">
+        <v>43556.601388888892</v>
+      </c>
+      <c r="D4126">
+        <v>0</v>
+      </c>
+      <c r="E4126">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4127" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4127" s="1">
+        <v>43556.611805555556</v>
+      </c>
+      <c r="D4127">
+        <v>0</v>
+      </c>
+      <c r="E4127">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4128" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4128" s="1">
+        <v>43556.612500000003</v>
+      </c>
+      <c r="D4128">
+        <v>1</v>
+      </c>
+      <c r="F4128">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4129" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4129" s="1">
+        <v>43556.62222222222</v>
+      </c>
+      <c r="D4129">
+        <v>0</v>
+      </c>
+      <c r="E4129">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4130" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4130" s="1">
+        <v>43556.632638888892</v>
+      </c>
+      <c r="D4130">
+        <v>0</v>
+      </c>
+      <c r="E4130">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4131" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4131" s="1">
+        <v>43556.652083333334</v>
+      </c>
+      <c r="D4131">
+        <v>1</v>
+      </c>
+      <c r="F4131">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated data, includes heartrate and reducose test.
</commit_message>
<xml_diff>
--- a/librelink/Librelink.xlsx
+++ b/librelink/Librelink.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sprague/OneDrive/Sprague 2019/Health 2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="13_ncr:1_{1DF15EB1-8D61-6642-9AC4-0A049F576367}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{A74ED3A2-9B31-764E-9931-5C709146D054}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{1DF15EB1-8D61-6642-9AC4-0A049F576367}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{AEBEACD1-FC73-FF48-B813-47DD138D8685}"/>
   <bookViews>
     <workbookView xWindow="13920" yWindow="1180" windowWidth="17400" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="68">
   <si>
     <t>Meter</t>
   </si>
@@ -229,6 +229,9 @@
   </si>
   <si>
     <t>Whole wheat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whole wheat bread w Reducose </t>
   </si>
 </sst>
 </file>
@@ -794,8 +797,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF602BB5-9469-1B45-BB1A-DFBEABAFCD1B}" name="Table1" displayName="Table1" ref="A1:S4198" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:S4198" xr:uid="{A8E95FAB-7D33-F24D-8350-CC174D759A60}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF602BB5-9469-1B45-BB1A-DFBEABAFCD1B}" name="Table1" displayName="Table1" ref="A1:S4259" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:S4259" xr:uid="{A8E95FAB-7D33-F24D-8350-CC174D759A60}"/>
   <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{374D21D6-0283-C44B-8028-4060CB201675}" name="Meter"/>
     <tableColumn id="2" xr3:uid="{48610F22-94E8-1142-AF15-100D6756BE81}" name="Serial Number"/>
@@ -1118,12 +1121,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S4198"/>
+  <dimension ref="A1:S4259"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4103" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A4226" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="C4132" sqref="C4132:G4198"/>
+      <selection pane="bottomLeft" activeCell="C4239" sqref="C4239:F4259"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -48943,6 +48946,677 @@
         <v>82</v>
       </c>
     </row>
+    <row r="4199" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4199" s="1">
+        <v>43557.27847222222</v>
+      </c>
+      <c r="D4199">
+        <v>1</v>
+      </c>
+      <c r="F4199">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4200" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4200" s="1">
+        <v>43557.284722222219</v>
+      </c>
+      <c r="D4200">
+        <v>0</v>
+      </c>
+      <c r="E4200">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4201" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4201" s="1">
+        <v>43557.295138888891</v>
+      </c>
+      <c r="D4201">
+        <v>0</v>
+      </c>
+      <c r="E4201">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4202" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4202" s="1">
+        <v>43557.305555555555</v>
+      </c>
+      <c r="D4202">
+        <v>0</v>
+      </c>
+      <c r="E4202">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4203" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4203" s="1">
+        <v>43557.315972222219</v>
+      </c>
+      <c r="D4203">
+        <v>0</v>
+      </c>
+      <c r="E4203">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4204" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4204" s="1">
+        <v>43557.326388888891</v>
+      </c>
+      <c r="D4204">
+        <v>0</v>
+      </c>
+      <c r="E4204">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4205" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4205" s="1">
+        <v>43557.337500000001</v>
+      </c>
+      <c r="D4205">
+        <v>0</v>
+      </c>
+      <c r="E4205">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4206" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4206" s="1">
+        <v>43557.343055555553</v>
+      </c>
+      <c r="D4206">
+        <v>1</v>
+      </c>
+      <c r="F4206">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4207" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4207" s="1">
+        <v>43557.347916666666</v>
+      </c>
+      <c r="D4207">
+        <v>0</v>
+      </c>
+      <c r="E4207">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4208" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4208" s="1">
+        <v>43557.352777777778</v>
+      </c>
+      <c r="D4208">
+        <v>1</v>
+      </c>
+      <c r="F4208">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4209" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4209" s="1">
+        <v>43557.35833333333</v>
+      </c>
+      <c r="D4209">
+        <v>0</v>
+      </c>
+      <c r="E4209">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4210" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4210" s="1">
+        <v>43557.368750000001</v>
+      </c>
+      <c r="D4210">
+        <v>0</v>
+      </c>
+      <c r="E4210">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4211" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4211" s="1">
+        <v>43557.379166666666</v>
+      </c>
+      <c r="D4211">
+        <v>0</v>
+      </c>
+      <c r="E4211">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4212" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4212" s="1">
+        <v>43557.38958333333</v>
+      </c>
+      <c r="D4212">
+        <v>0</v>
+      </c>
+      <c r="E4212">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4213" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4213" s="1">
+        <v>43557.4</v>
+      </c>
+      <c r="D4213">
+        <v>0</v>
+      </c>
+      <c r="E4213">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4214" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4214" s="1">
+        <v>43557.411111111112</v>
+      </c>
+      <c r="D4214">
+        <v>0</v>
+      </c>
+      <c r="E4214">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4215" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4215" s="1">
+        <v>43557.418749999997</v>
+      </c>
+      <c r="D4215">
+        <v>1</v>
+      </c>
+      <c r="F4215">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4216" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4216" s="1">
+        <v>43557.421527777777</v>
+      </c>
+      <c r="D4216">
+        <v>0</v>
+      </c>
+      <c r="E4216">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4217" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4217" s="1">
+        <v>43557.431944444441</v>
+      </c>
+      <c r="D4217">
+        <v>0</v>
+      </c>
+      <c r="E4217">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4218" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4218" s="1">
+        <v>43557.43472222222</v>
+      </c>
+      <c r="D4218">
+        <v>1</v>
+      </c>
+      <c r="F4218">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4219" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4219" s="1">
+        <v>43557.442361111112</v>
+      </c>
+      <c r="D4219">
+        <v>0</v>
+      </c>
+      <c r="E4219">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4220" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4220" s="1">
+        <v>43557.452777777777</v>
+      </c>
+      <c r="D4220">
+        <v>0</v>
+      </c>
+      <c r="E4220">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4221" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4221" s="1">
+        <v>43557.463888888888</v>
+      </c>
+      <c r="D4221">
+        <v>0</v>
+      </c>
+      <c r="E4221">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4222" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4222" s="1">
+        <v>43557.472916666666</v>
+      </c>
+      <c r="D4222">
+        <v>1</v>
+      </c>
+      <c r="F4222">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4223" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4223" s="1">
+        <v>43557.472916666666</v>
+      </c>
+      <c r="D4223">
+        <v>6</v>
+      </c>
+      <c r="N4223" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4224" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4224" s="1">
+        <v>43557.474305555559</v>
+      </c>
+      <c r="D4224">
+        <v>0</v>
+      </c>
+      <c r="E4224">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4225" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4225" s="1">
+        <v>43557.484722222223</v>
+      </c>
+      <c r="D4225">
+        <v>0</v>
+      </c>
+      <c r="E4225">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4226" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4226" s="1">
+        <v>43557.495138888888</v>
+      </c>
+      <c r="D4226">
+        <v>0</v>
+      </c>
+      <c r="E4226">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4227" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4227" s="1">
+        <v>43557.497916666667</v>
+      </c>
+      <c r="D4227">
+        <v>1</v>
+      </c>
+      <c r="F4227">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4228" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4228" s="1">
+        <v>43557.505555555559</v>
+      </c>
+      <c r="D4228">
+        <v>0</v>
+      </c>
+      <c r="E4228">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4229" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4229" s="1">
+        <v>43557.505555555559</v>
+      </c>
+      <c r="D4229">
+        <v>1</v>
+      </c>
+      <c r="F4229">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4230" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4230" s="1">
+        <v>43557.513888888891</v>
+      </c>
+      <c r="D4230">
+        <v>1</v>
+      </c>
+      <c r="F4230">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4231" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4231" s="1">
+        <v>43557.515972222223</v>
+      </c>
+      <c r="D4231">
+        <v>0</v>
+      </c>
+      <c r="E4231">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4232" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4232" s="1">
+        <v>43557.521527777775</v>
+      </c>
+      <c r="D4232">
+        <v>1</v>
+      </c>
+      <c r="F4232">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4233" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4233" s="1">
+        <v>43557.527083333334</v>
+      </c>
+      <c r="D4233">
+        <v>0</v>
+      </c>
+      <c r="E4233">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4234" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4234" s="1">
+        <v>43557.531944444447</v>
+      </c>
+      <c r="D4234">
+        <v>1</v>
+      </c>
+      <c r="F4234">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4235" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4235" s="1">
+        <v>43557.536805555559</v>
+      </c>
+      <c r="D4235">
+        <v>0</v>
+      </c>
+      <c r="E4235">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4236" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4236" s="1">
+        <v>43557.544444444444</v>
+      </c>
+      <c r="D4236">
+        <v>1</v>
+      </c>
+      <c r="F4236">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4237" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4237" s="1">
+        <v>43557.549305555556</v>
+      </c>
+      <c r="D4237">
+        <v>1</v>
+      </c>
+      <c r="F4237">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4238" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4238" s="1">
+        <v>43557.550694444442</v>
+      </c>
+      <c r="D4238">
+        <v>1</v>
+      </c>
+      <c r="F4238">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4239" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4239" s="1">
+        <v>43557.556944444441</v>
+      </c>
+      <c r="D4239">
+        <v>1</v>
+      </c>
+      <c r="F4239">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4240" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4240" s="1">
+        <v>43557.557638888888</v>
+      </c>
+      <c r="D4240">
+        <v>0</v>
+      </c>
+      <c r="E4240">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4241" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4241" s="1">
+        <v>43557.568055555559</v>
+      </c>
+      <c r="D4241">
+        <v>0</v>
+      </c>
+      <c r="E4241">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4242" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4242" s="1">
+        <v>43557.578472222223</v>
+      </c>
+      <c r="D4242">
+        <v>0</v>
+      </c>
+      <c r="E4242">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4243" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4243" s="1">
+        <v>43557.586111111108</v>
+      </c>
+      <c r="D4243">
+        <v>1</v>
+      </c>
+      <c r="F4243">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4244" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4244" s="1">
+        <v>43557.589583333334</v>
+      </c>
+      <c r="D4244">
+        <v>0</v>
+      </c>
+      <c r="E4244">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4245" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4245" s="1">
+        <v>43557.593055555553</v>
+      </c>
+      <c r="D4245">
+        <v>1</v>
+      </c>
+      <c r="F4245">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4246" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4246" s="1">
+        <v>43557.599999999999</v>
+      </c>
+      <c r="D4246">
+        <v>1</v>
+      </c>
+      <c r="F4246">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4247" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4247" s="1">
+        <v>43557.601388888892</v>
+      </c>
+      <c r="D4247">
+        <v>0</v>
+      </c>
+      <c r="E4247">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4248" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4248" s="1">
+        <v>43557.611805555556</v>
+      </c>
+      <c r="D4248">
+        <v>0</v>
+      </c>
+      <c r="E4248">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4249" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4249" s="1">
+        <v>43557.62222222222</v>
+      </c>
+      <c r="D4249">
+        <v>0</v>
+      </c>
+      <c r="E4249">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4250" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4250" s="1">
+        <v>43557.632638888892</v>
+      </c>
+      <c r="D4250">
+        <v>0</v>
+      </c>
+      <c r="E4250">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4251" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4251" s="1">
+        <v>43557.643055555556</v>
+      </c>
+      <c r="D4251">
+        <v>0</v>
+      </c>
+      <c r="E4251">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4252" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4252" s="1">
+        <v>43557.65347222222</v>
+      </c>
+      <c r="D4252">
+        <v>0</v>
+      </c>
+      <c r="E4252">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4253" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4253" s="1">
+        <v>43557.663888888892</v>
+      </c>
+      <c r="D4253">
+        <v>0</v>
+      </c>
+      <c r="E4253">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4254" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4254" s="1">
+        <v>43557.674305555556</v>
+      </c>
+      <c r="D4254">
+        <v>0</v>
+      </c>
+      <c r="E4254">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4255" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4255" s="1">
+        <v>43557.68472222222</v>
+      </c>
+      <c r="D4255">
+        <v>0</v>
+      </c>
+      <c r="E4255">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4256" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4256" s="1">
+        <v>43557.695138888892</v>
+      </c>
+      <c r="D4256">
+        <v>0</v>
+      </c>
+      <c r="E4256">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4257" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4257" s="1">
+        <v>43557.700694444444</v>
+      </c>
+      <c r="D4257">
+        <v>1</v>
+      </c>
+      <c r="F4257">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4258" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4258" s="1">
+        <v>43557.705555555556</v>
+      </c>
+      <c r="D4258">
+        <v>0</v>
+      </c>
+      <c r="E4258">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4259" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4259" s="1">
+        <v>43557.718055555553</v>
+      </c>
+      <c r="D4259">
+        <v>1</v>
+      </c>
+      <c r="F4259">
+        <v>83</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Input by date instead of range. Updated data thru morning Apr 3
</commit_message>
<xml_diff>
--- a/librelink/Librelink.xlsx
+++ b/librelink/Librelink.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sprague/OneDrive/Sprague 2019/Health 2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{1DF15EB1-8D61-6642-9AC4-0A049F576367}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{AEBEACD1-FC73-FF48-B813-47DD138D8685}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:1_{1DF15EB1-8D61-6642-9AC4-0A049F576367}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{03B012FB-06DC-A34B-99AA-8406D9143EE1}"/>
   <bookViews>
     <workbookView xWindow="13920" yWindow="1180" windowWidth="17400" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="70">
   <si>
     <t>Meter</t>
   </si>
@@ -232,6 +232,12 @@
   </si>
   <si>
     <t xml:space="preserve">Whole wheat bread w Reducose </t>
+  </si>
+  <si>
+    <t>Nuts</t>
+  </si>
+  <si>
+    <t>Pasta cheese bread salad</t>
   </si>
 </sst>
 </file>
@@ -797,8 +803,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF602BB5-9469-1B45-BB1A-DFBEABAFCD1B}" name="Table1" displayName="Table1" ref="A1:S4259" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:S4259" xr:uid="{A8E95FAB-7D33-F24D-8350-CC174D759A60}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF602BB5-9469-1B45-BB1A-DFBEABAFCD1B}" name="Table1" displayName="Table1" ref="A1:S4316" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:S4316" xr:uid="{A8E95FAB-7D33-F24D-8350-CC174D759A60}"/>
   <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{374D21D6-0283-C44B-8028-4060CB201675}" name="Meter"/>
     <tableColumn id="2" xr3:uid="{48610F22-94E8-1142-AF15-100D6756BE81}" name="Serial Number"/>
@@ -1121,12 +1127,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S4259"/>
+  <dimension ref="A1:S4316"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4226" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A4234" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="C4239" sqref="C4239:F4259"/>
+      <selection pane="bottomLeft" activeCell="C4260" sqref="C4260:N4316"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -49584,7 +49590,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4257" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="4257" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C4257" s="1">
         <v>43557.700694444444</v>
       </c>
@@ -49595,7 +49601,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4258" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="4258" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C4258" s="1">
         <v>43557.705555555556</v>
       </c>
@@ -49606,7 +49612,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4259" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="4259" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C4259" s="1">
         <v>43557.718055555553</v>
       </c>
@@ -49615,6 +49621,633 @@
       </c>
       <c r="F4259">
         <v>83</v>
+      </c>
+    </row>
+    <row r="4260" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4260" s="1">
+        <v>43557.718055555553</v>
+      </c>
+      <c r="D4260">
+        <v>6</v>
+      </c>
+      <c r="N4260" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4261" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4261" s="1">
+        <v>43557.726388888892</v>
+      </c>
+      <c r="D4261">
+        <v>0</v>
+      </c>
+      <c r="E4261">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4262" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4262" s="1">
+        <v>43557.736805555556</v>
+      </c>
+      <c r="D4262">
+        <v>0</v>
+      </c>
+      <c r="E4262">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4263" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4263" s="1">
+        <v>43557.748611111114</v>
+      </c>
+      <c r="D4263">
+        <v>0</v>
+      </c>
+      <c r="E4263">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4264" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4264" s="1">
+        <v>43557.751388888886</v>
+      </c>
+      <c r="D4264">
+        <v>1</v>
+      </c>
+      <c r="F4264">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4265" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4265" s="1">
+        <v>43557.759027777778</v>
+      </c>
+      <c r="D4265">
+        <v>0</v>
+      </c>
+      <c r="E4265">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4266" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4266" s="1">
+        <v>43557.769444444442</v>
+      </c>
+      <c r="D4266">
+        <v>0</v>
+      </c>
+      <c r="E4266">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4267" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4267" s="1">
+        <v>43557.779861111114</v>
+      </c>
+      <c r="D4267">
+        <v>0</v>
+      </c>
+      <c r="E4267">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4268" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4268" s="1">
+        <v>43557.790277777778</v>
+      </c>
+      <c r="D4268">
+        <v>0</v>
+      </c>
+      <c r="E4268">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4269" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4269" s="1">
+        <v>43557.800694444442</v>
+      </c>
+      <c r="D4269">
+        <v>0</v>
+      </c>
+      <c r="E4269">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4270" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4270" s="1">
+        <v>43557.811111111114</v>
+      </c>
+      <c r="D4270">
+        <v>0</v>
+      </c>
+      <c r="E4270">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4271" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4271" s="1">
+        <v>43557.821527777778</v>
+      </c>
+      <c r="D4271">
+        <v>0</v>
+      </c>
+      <c r="E4271">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4272" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4272" s="1">
+        <v>43557.831944444442</v>
+      </c>
+      <c r="D4272">
+        <v>0</v>
+      </c>
+      <c r="E4272">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4273" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4273" s="1">
+        <v>43557.842361111114</v>
+      </c>
+      <c r="D4273">
+        <v>0</v>
+      </c>
+      <c r="E4273">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4274" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4274" s="1">
+        <v>43557.852777777778</v>
+      </c>
+      <c r="D4274">
+        <v>0</v>
+      </c>
+      <c r="E4274">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4275" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4275" s="1">
+        <v>43557.863194444442</v>
+      </c>
+      <c r="D4275">
+        <v>0</v>
+      </c>
+      <c r="E4275">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4276" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4276" s="1">
+        <v>43557.873611111114</v>
+      </c>
+      <c r="D4276">
+        <v>0</v>
+      </c>
+      <c r="E4276">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4277" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4277" s="1">
+        <v>43557.884027777778</v>
+      </c>
+      <c r="D4277">
+        <v>0</v>
+      </c>
+      <c r="E4277">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4278" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4278" s="1">
+        <v>43557.886805555558</v>
+      </c>
+      <c r="D4278">
+        <v>1</v>
+      </c>
+      <c r="F4278">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4279" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4279" s="1">
+        <v>43557.886805555558</v>
+      </c>
+      <c r="D4279">
+        <v>6</v>
+      </c>
+      <c r="N4279" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4280" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4280" s="1">
+        <v>43557.895138888889</v>
+      </c>
+      <c r="D4280">
+        <v>0</v>
+      </c>
+      <c r="E4280">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4281" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4281" s="1">
+        <v>43557.897222222222</v>
+      </c>
+      <c r="D4281">
+        <v>1</v>
+      </c>
+      <c r="F4281">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4282" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4282" s="1">
+        <v>43557.905555555553</v>
+      </c>
+      <c r="D4282">
+        <v>0</v>
+      </c>
+      <c r="E4282">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4283" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4283" s="1">
+        <v>43557.925694444442</v>
+      </c>
+      <c r="D4283">
+        <v>1</v>
+      </c>
+      <c r="F4283">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4284" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4284" s="1">
+        <v>43557.97152777778</v>
+      </c>
+      <c r="D4284">
+        <v>0</v>
+      </c>
+      <c r="E4284">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4285" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4285" s="1">
+        <v>43557.981944444444</v>
+      </c>
+      <c r="D4285">
+        <v>0</v>
+      </c>
+      <c r="E4285">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4286" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4286" s="1">
+        <v>43557.992361111108</v>
+      </c>
+      <c r="D4286">
+        <v>0</v>
+      </c>
+      <c r="E4286">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4287" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4287" s="1">
+        <v>43558.00277777778</v>
+      </c>
+      <c r="D4287">
+        <v>0</v>
+      </c>
+      <c r="E4287">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4288" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4288" s="1">
+        <v>43558.013194444444</v>
+      </c>
+      <c r="D4288">
+        <v>0</v>
+      </c>
+      <c r="E4288">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4289" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4289" s="1">
+        <v>43558.023611111108</v>
+      </c>
+      <c r="D4289">
+        <v>0</v>
+      </c>
+      <c r="E4289">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4290" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4290" s="1">
+        <v>43558.03402777778</v>
+      </c>
+      <c r="D4290">
+        <v>0</v>
+      </c>
+      <c r="E4290">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4291" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4291" s="1">
+        <v>43558.044444444444</v>
+      </c>
+      <c r="D4291">
+        <v>0</v>
+      </c>
+      <c r="E4291">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4292" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4292" s="1">
+        <v>43558.054861111108</v>
+      </c>
+      <c r="D4292">
+        <v>0</v>
+      </c>
+      <c r="E4292">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4293" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4293" s="1">
+        <v>43558.06527777778</v>
+      </c>
+      <c r="D4293">
+        <v>0</v>
+      </c>
+      <c r="E4293">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4294" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4294" s="1">
+        <v>43558.075694444444</v>
+      </c>
+      <c r="D4294">
+        <v>0</v>
+      </c>
+      <c r="E4294">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4295" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4295" s="1">
+        <v>43558.086111111108</v>
+      </c>
+      <c r="D4295">
+        <v>0</v>
+      </c>
+      <c r="E4295">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4296" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4296" s="1">
+        <v>43558.09652777778</v>
+      </c>
+      <c r="D4296">
+        <v>0</v>
+      </c>
+      <c r="E4296">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4297" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4297" s="1">
+        <v>43558.106944444444</v>
+      </c>
+      <c r="D4297">
+        <v>0</v>
+      </c>
+      <c r="E4297">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4298" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4298" s="1">
+        <v>43558.117361111108</v>
+      </c>
+      <c r="D4298">
+        <v>0</v>
+      </c>
+      <c r="E4298">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4299" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4299" s="1">
+        <v>43558.12777777778</v>
+      </c>
+      <c r="D4299">
+        <v>0</v>
+      </c>
+      <c r="E4299">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4300" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4300" s="1">
+        <v>43558.138194444444</v>
+      </c>
+      <c r="D4300">
+        <v>0</v>
+      </c>
+      <c r="E4300">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4301" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4301" s="1">
+        <v>43558.148611111108</v>
+      </c>
+      <c r="D4301">
+        <v>0</v>
+      </c>
+      <c r="E4301">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4302" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4302" s="1">
+        <v>43558.15902777778</v>
+      </c>
+      <c r="D4302">
+        <v>0</v>
+      </c>
+      <c r="E4302">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4303" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4303" s="1">
+        <v>43558.169444444444</v>
+      </c>
+      <c r="D4303">
+        <v>0</v>
+      </c>
+      <c r="E4303">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4304" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4304" s="1">
+        <v>43558.179861111108</v>
+      </c>
+      <c r="D4304">
+        <v>0</v>
+      </c>
+      <c r="E4304">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4305" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4305" s="1">
+        <v>43558.19027777778</v>
+      </c>
+      <c r="D4305">
+        <v>0</v>
+      </c>
+      <c r="E4305">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4306" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4306" s="1">
+        <v>43558.200694444444</v>
+      </c>
+      <c r="D4306">
+        <v>0</v>
+      </c>
+      <c r="E4306">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4307" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4307" s="1">
+        <v>43558.211111111108</v>
+      </c>
+      <c r="D4307">
+        <v>0</v>
+      </c>
+      <c r="E4307">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4308" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4308" s="1">
+        <v>43558.22152777778</v>
+      </c>
+      <c r="D4308">
+        <v>0</v>
+      </c>
+      <c r="E4308">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4309" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4309" s="1">
+        <v>43558.231944444444</v>
+      </c>
+      <c r="D4309">
+        <v>0</v>
+      </c>
+      <c r="E4309">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4310" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4310" s="1">
+        <v>43558.242361111108</v>
+      </c>
+      <c r="D4310">
+        <v>0</v>
+      </c>
+      <c r="E4310">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4311" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4311" s="1">
+        <v>43558.25277777778</v>
+      </c>
+      <c r="D4311">
+        <v>0</v>
+      </c>
+      <c r="E4311">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4312" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4312" s="1">
+        <v>43558.263194444444</v>
+      </c>
+      <c r="D4312">
+        <v>0</v>
+      </c>
+      <c r="E4312">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4313" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4313" s="1">
+        <v>43558.273611111108</v>
+      </c>
+      <c r="D4313">
+        <v>0</v>
+      </c>
+      <c r="E4313">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4314" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4314" s="1">
+        <v>43558.28402777778</v>
+      </c>
+      <c r="D4314">
+        <v>0</v>
+      </c>
+      <c r="E4314">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4315" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4315" s="1">
+        <v>43558.302083333336</v>
+      </c>
+      <c r="D4315">
+        <v>1</v>
+      </c>
+      <c r="F4315">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4316" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4316" s="1">
+        <v>43558.304166666669</v>
+      </c>
+      <c r="D4316">
+        <v>1</v>
+      </c>
+      <c r="F4316">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Latest data 2019-04-05 am
</commit_message>
<xml_diff>
--- a/librelink/Librelink.xlsx
+++ b/librelink/Librelink.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sprague/OneDrive/Sprague 2019/Health 2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:1_{1DF15EB1-8D61-6642-9AC4-0A049F576367}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{03B012FB-06DC-A34B-99AA-8406D9143EE1}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="13_ncr:1_{1DF15EB1-8D61-6642-9AC4-0A049F576367}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{874CB720-4375-C943-9793-167910174A6D}"/>
   <bookViews>
-    <workbookView xWindow="13920" yWindow="1180" windowWidth="17400" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8380" yWindow="1100" windowWidth="17400" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Librelink" sheetId="1" r:id="rId1"/>
@@ -803,8 +803,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF602BB5-9469-1B45-BB1A-DFBEABAFCD1B}" name="Table1" displayName="Table1" ref="A1:S4316" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:S4316" xr:uid="{A8E95FAB-7D33-F24D-8350-CC174D759A60}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF602BB5-9469-1B45-BB1A-DFBEABAFCD1B}" name="Table1" displayName="Table1" ref="A1:S4364" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:S4364" xr:uid="{A8E95FAB-7D33-F24D-8350-CC174D759A60}"/>
   <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{374D21D6-0283-C44B-8028-4060CB201675}" name="Meter"/>
     <tableColumn id="2" xr3:uid="{48610F22-94E8-1142-AF15-100D6756BE81}" name="Serial Number"/>
@@ -1127,12 +1127,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S4316"/>
+  <dimension ref="A1:S4364"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4234" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A4344" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="C4260" sqref="C4260:N4316"/>
+      <selection pane="bottomLeft" activeCell="N4358" sqref="N4358"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -50250,6 +50250,540 @@
         <v>81</v>
       </c>
     </row>
+    <row r="4317" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4317" s="1">
+        <v>43558.306944444441</v>
+      </c>
+      <c r="D4317">
+        <v>0</v>
+      </c>
+      <c r="E4317">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4318" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4318" s="1">
+        <v>43558.317361111112</v>
+      </c>
+      <c r="D4318">
+        <v>0</v>
+      </c>
+      <c r="E4318">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4319" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4319" s="1">
+        <v>43558.327777777777</v>
+      </c>
+      <c r="D4319">
+        <v>0</v>
+      </c>
+      <c r="E4319">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4320" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4320" s="1">
+        <v>43558.338194444441</v>
+      </c>
+      <c r="D4320">
+        <v>0</v>
+      </c>
+      <c r="E4320">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4321" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4321" s="1">
+        <v>43558.348611111112</v>
+      </c>
+      <c r="D4321">
+        <v>0</v>
+      </c>
+      <c r="E4321">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4322" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4322" s="1">
+        <v>43558.359027777777</v>
+      </c>
+      <c r="D4322">
+        <v>0</v>
+      </c>
+      <c r="E4322">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4323" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4323" s="1">
+        <v>43558.369444444441</v>
+      </c>
+      <c r="D4323">
+        <v>0</v>
+      </c>
+      <c r="E4323">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4324" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4324" s="1">
+        <v>43558.379861111112</v>
+      </c>
+      <c r="D4324">
+        <v>0</v>
+      </c>
+      <c r="E4324">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4325" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4325" s="1">
+        <v>43558.390277777777</v>
+      </c>
+      <c r="D4325">
+        <v>0</v>
+      </c>
+      <c r="E4325">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4326" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4326" s="1">
+        <v>43558.400694444441</v>
+      </c>
+      <c r="D4326">
+        <v>0</v>
+      </c>
+      <c r="E4326">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4327" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4327" s="1">
+        <v>43558.411111111112</v>
+      </c>
+      <c r="D4327">
+        <v>0</v>
+      </c>
+      <c r="E4327">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4328" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4328" s="1">
+        <v>43558.421527777777</v>
+      </c>
+      <c r="D4328">
+        <v>0</v>
+      </c>
+      <c r="E4328">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4329" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4329" s="1">
+        <v>43558.431944444441</v>
+      </c>
+      <c r="D4329">
+        <v>0</v>
+      </c>
+      <c r="E4329">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4330" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4330" s="1">
+        <v>43558.442361111112</v>
+      </c>
+      <c r="D4330">
+        <v>0</v>
+      </c>
+      <c r="E4330">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4331" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4331" s="1">
+        <v>43558.452777777777</v>
+      </c>
+      <c r="D4331">
+        <v>0</v>
+      </c>
+      <c r="E4331">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4332" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4332" s="1">
+        <v>43558.463194444441</v>
+      </c>
+      <c r="D4332">
+        <v>0</v>
+      </c>
+      <c r="E4332">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4333" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4333" s="1">
+        <v>43558.473611111112</v>
+      </c>
+      <c r="D4333">
+        <v>0</v>
+      </c>
+      <c r="E4333">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4334" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4334" s="1">
+        <v>43558.484027777777</v>
+      </c>
+      <c r="D4334">
+        <v>0</v>
+      </c>
+      <c r="E4334">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4335" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4335" s="1">
+        <v>43558.495138888888</v>
+      </c>
+      <c r="D4335">
+        <v>0</v>
+      </c>
+      <c r="E4335">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4336" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4336" s="1">
+        <v>43558.502083333333</v>
+      </c>
+      <c r="D4336">
+        <v>1</v>
+      </c>
+      <c r="F4336">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4337" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4337" s="1">
+        <v>43558.505555555559</v>
+      </c>
+      <c r="D4337">
+        <v>0</v>
+      </c>
+      <c r="E4337">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4338" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4338" s="1">
+        <v>43558.515972222223</v>
+      </c>
+      <c r="D4338">
+        <v>0</v>
+      </c>
+      <c r="E4338">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4339" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4339" s="1">
+        <v>43558.526388888888</v>
+      </c>
+      <c r="D4339">
+        <v>0</v>
+      </c>
+      <c r="E4339">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4340" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4340" s="1">
+        <v>43558.536805555559</v>
+      </c>
+      <c r="D4340">
+        <v>0</v>
+      </c>
+      <c r="E4340">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4341" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4341" s="1">
+        <v>43558.547222222223</v>
+      </c>
+      <c r="D4341">
+        <v>0</v>
+      </c>
+      <c r="E4341">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4342" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4342" s="1">
+        <v>43558.557638888888</v>
+      </c>
+      <c r="D4342">
+        <v>0</v>
+      </c>
+      <c r="E4342">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4343" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4343" s="1">
+        <v>43558.568055555559</v>
+      </c>
+      <c r="D4343">
+        <v>0</v>
+      </c>
+      <c r="E4343">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4344" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4344" s="1">
+        <v>43558.578472222223</v>
+      </c>
+      <c r="D4344">
+        <v>0</v>
+      </c>
+      <c r="E4344">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4345" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4345" s="1">
+        <v>43558.588888888888</v>
+      </c>
+      <c r="D4345">
+        <v>0</v>
+      </c>
+      <c r="E4345">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4346" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4346" s="1">
+        <v>43558.599305555559</v>
+      </c>
+      <c r="D4346">
+        <v>0</v>
+      </c>
+      <c r="E4346">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4347" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4347" s="1">
+        <v>43558.61041666667</v>
+      </c>
+      <c r="D4347">
+        <v>1</v>
+      </c>
+      <c r="F4347">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4348" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4348" s="1">
+        <v>43558.61041666667</v>
+      </c>
+      <c r="D4348">
+        <v>0</v>
+      </c>
+      <c r="E4348">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4349" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4349" s="1">
+        <v>43558.620833333334</v>
+      </c>
+      <c r="D4349">
+        <v>0</v>
+      </c>
+      <c r="E4349">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4350" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4350" s="1">
+        <v>43558.631249999999</v>
+      </c>
+      <c r="D4350">
+        <v>0</v>
+      </c>
+      <c r="E4350">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4351" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4351" s="1">
+        <v>43558.64166666667</v>
+      </c>
+      <c r="D4351">
+        <v>0</v>
+      </c>
+      <c r="E4351">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4352" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4352" s="1">
+        <v>43558.652777777781</v>
+      </c>
+      <c r="D4352">
+        <v>0</v>
+      </c>
+      <c r="E4352">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4353" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4353" s="1">
+        <v>43558.65902777778</v>
+      </c>
+      <c r="D4353">
+        <v>1</v>
+      </c>
+      <c r="F4353">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4354" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4354" s="1">
+        <v>43558.661111111112</v>
+      </c>
+      <c r="D4354">
+        <v>1</v>
+      </c>
+      <c r="F4354">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4355" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4355" s="1">
+        <v>43558.663194444445</v>
+      </c>
+      <c r="D4355">
+        <v>0</v>
+      </c>
+      <c r="E4355">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4356" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4356" s="1">
+        <v>43558.673611111109</v>
+      </c>
+      <c r="D4356">
+        <v>0</v>
+      </c>
+      <c r="E4356">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4357" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4357" s="1">
+        <v>43558.684027777781</v>
+      </c>
+      <c r="D4357">
+        <v>0</v>
+      </c>
+      <c r="E4357">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4358" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4358" s="1">
+        <v>43558.694444444445</v>
+      </c>
+      <c r="D4358">
+        <v>0</v>
+      </c>
+      <c r="E4358">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4359" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4359" s="1">
+        <v>43558.704861111109</v>
+      </c>
+      <c r="D4359">
+        <v>0</v>
+      </c>
+      <c r="E4359">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4360" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4360" s="1">
+        <v>43558.711805555555</v>
+      </c>
+      <c r="D4360">
+        <v>1</v>
+      </c>
+      <c r="F4360">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4361" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4361" s="1">
+        <v>43558.716666666667</v>
+      </c>
+      <c r="D4361">
+        <v>1</v>
+      </c>
+      <c r="F4361">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4362" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4362" s="1">
+        <v>43558.716666666667</v>
+      </c>
+      <c r="D4362">
+        <v>1</v>
+      </c>
+      <c r="F4362" s="3">
+        <v>93</v>
+      </c>
+      <c r="N4362">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4363" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4363" s="1">
+        <v>43558.723611111112</v>
+      </c>
+      <c r="D4363">
+        <v>1</v>
+      </c>
+      <c r="F4363">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4364" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4364" s="1">
+        <v>43558.723611111112</v>
+      </c>
+      <c r="D4364">
+        <v>1</v>
+      </c>
+      <c r="F4364" s="3">
+        <v>100</v>
+      </c>
+      <c r="N4364">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Updates for 2019-04-06 am
</commit_message>
<xml_diff>
--- a/librelink/Librelink.xlsx
+++ b/librelink/Librelink.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sprague/OneDrive/Sprague 2019/Health 2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="13_ncr:1_{1DF15EB1-8D61-6642-9AC4-0A049F576367}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{874CB720-4375-C943-9793-167910174A6D}"/>
+  <xr:revisionPtr revIDLastSave="160" documentId="13_ncr:1_{1DF15EB1-8D61-6642-9AC4-0A049F576367}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{909B392B-EC6A-1B4A-92EA-06FBAECCE476}"/>
   <bookViews>
-    <workbookView xWindow="8380" yWindow="1100" windowWidth="17400" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11260" yWindow="1360" windowWidth="17400" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Librelink" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="72">
   <si>
     <t>Meter</t>
   </si>
@@ -238,6 +238,12 @@
   </si>
   <si>
     <t>Pasta cheese bread salad</t>
+  </si>
+  <si>
+    <t>86 whole wheat bread</t>
+  </si>
+  <si>
+    <t>Blueberry kefir</t>
   </si>
 </sst>
 </file>
@@ -803,8 +809,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF602BB5-9469-1B45-BB1A-DFBEABAFCD1B}" name="Table1" displayName="Table1" ref="A1:S4364" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:S4364" xr:uid="{A8E95FAB-7D33-F24D-8350-CC174D759A60}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF602BB5-9469-1B45-BB1A-DFBEABAFCD1B}" name="Table1" displayName="Table1" ref="A1:S4678" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:S4678" xr:uid="{A8E95FAB-7D33-F24D-8350-CC174D759A60}"/>
   <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{374D21D6-0283-C44B-8028-4060CB201675}" name="Meter"/>
     <tableColumn id="2" xr3:uid="{48610F22-94E8-1142-AF15-100D6756BE81}" name="Serial Number"/>
@@ -1127,12 +1133,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S4364"/>
+  <dimension ref="A1:S4678"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4344" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A4652" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="N4358" sqref="N4358"/>
+      <selection pane="bottomLeft" activeCell="I4663" sqref="I4663"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -50646,7 +50652,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4353" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="4353" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C4353" s="1">
         <v>43558.65902777778</v>
       </c>
@@ -50657,7 +50663,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4354" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="4354" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C4354" s="1">
         <v>43558.661111111112</v>
       </c>
@@ -50668,7 +50674,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4355" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="4355" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C4355" s="1">
         <v>43558.663194444445</v>
       </c>
@@ -50679,7 +50685,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4356" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="4356" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C4356" s="1">
         <v>43558.673611111109</v>
       </c>
@@ -50690,7 +50696,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4357" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="4357" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C4357" s="1">
         <v>43558.684027777781</v>
       </c>
@@ -50701,7 +50707,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4358" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="4358" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C4358" s="1">
         <v>43558.694444444445</v>
       </c>
@@ -50712,7 +50718,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4359" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="4359" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C4359" s="1">
         <v>43558.704861111109</v>
       </c>
@@ -50723,7 +50729,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4360" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="4360" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C4360" s="1">
         <v>43558.711805555555</v>
       </c>
@@ -50734,7 +50740,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4361" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="4361" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C4361" s="1">
         <v>43558.716666666667</v>
       </c>
@@ -50745,7 +50751,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4362" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="4362" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C4362" s="1">
         <v>43558.716666666667</v>
       </c>
@@ -50753,13 +50759,16 @@
         <v>1</v>
       </c>
       <c r="F4362" s="3">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="N4362">
         <v>93</v>
       </c>
-    </row>
-    <row r="4363" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="O4362">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4363" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C4363" s="1">
         <v>43558.723611111112</v>
       </c>
@@ -50770,7 +50779,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4364" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="4364" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C4364" s="1">
         <v>43558.723611111112</v>
       </c>
@@ -50778,10 +50787,3569 @@
         <v>1</v>
       </c>
       <c r="F4364" s="3">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="N4364">
         <v>100</v>
+      </c>
+      <c r="O4364">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4365" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4365" s="1">
+        <v>43558.725694444445</v>
+      </c>
+      <c r="D4365">
+        <v>0</v>
+      </c>
+      <c r="E4365">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4366" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4366" s="1">
+        <v>43558.736111111109</v>
+      </c>
+      <c r="D4366">
+        <v>0</v>
+      </c>
+      <c r="E4366">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4367" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4367" s="1">
+        <v>43558.746527777781</v>
+      </c>
+      <c r="D4367">
+        <v>0</v>
+      </c>
+      <c r="E4367">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4368" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4368" s="1">
+        <v>43558.756944444445</v>
+      </c>
+      <c r="D4368">
+        <v>0</v>
+      </c>
+      <c r="E4368">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4369" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4369" s="1">
+        <v>43558.767361111109</v>
+      </c>
+      <c r="D4369">
+        <v>0</v>
+      </c>
+      <c r="E4369">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4370" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4370" s="1">
+        <v>43558.777777777781</v>
+      </c>
+      <c r="D4370">
+        <v>0</v>
+      </c>
+      <c r="E4370">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4371" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4371" s="1">
+        <v>43558.788888888892</v>
+      </c>
+      <c r="D4371">
+        <v>0</v>
+      </c>
+      <c r="E4371">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4372" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4372" s="1">
+        <v>43558.790277777778</v>
+      </c>
+      <c r="D4372">
+        <v>1</v>
+      </c>
+      <c r="F4372">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4373" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4373" s="1">
+        <v>43558.795138888891</v>
+      </c>
+      <c r="D4373">
+        <v>1</v>
+      </c>
+      <c r="F4373">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4374" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4374" s="1">
+        <v>43558.797222222223</v>
+      </c>
+      <c r="D4374">
+        <v>1</v>
+      </c>
+      <c r="F4374">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4375" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4375" s="1">
+        <v>43558.797222222223</v>
+      </c>
+      <c r="D4375">
+        <v>1</v>
+      </c>
+      <c r="F4375" s="3">
+        <v>74</v>
+      </c>
+      <c r="N4375">
+        <v>84</v>
+      </c>
+      <c r="O4375">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4376" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4376" s="1">
+        <v>43558.799305555556</v>
+      </c>
+      <c r="D4376">
+        <v>0</v>
+      </c>
+      <c r="E4376">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4377" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4377" s="1">
+        <v>43558.810416666667</v>
+      </c>
+      <c r="D4377">
+        <v>0</v>
+      </c>
+      <c r="E4377">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4378" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4378" s="1">
+        <v>43558.813194444447</v>
+      </c>
+      <c r="D4378">
+        <v>1</v>
+      </c>
+      <c r="F4378">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4379" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4379" s="1">
+        <v>43558.820833333331</v>
+      </c>
+      <c r="D4379">
+        <v>0</v>
+      </c>
+      <c r="E4379">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4380" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4380" s="1">
+        <v>43558.831250000003</v>
+      </c>
+      <c r="D4380">
+        <v>0</v>
+      </c>
+      <c r="E4380">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4381" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4381" s="1">
+        <v>43558.841666666667</v>
+      </c>
+      <c r="D4381">
+        <v>0</v>
+      </c>
+      <c r="E4381">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4382" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4382" s="1">
+        <v>43558.852083333331</v>
+      </c>
+      <c r="D4382">
+        <v>0</v>
+      </c>
+      <c r="E4382">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4383" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4383" s="1">
+        <v>43558.862500000003</v>
+      </c>
+      <c r="D4383">
+        <v>0</v>
+      </c>
+      <c r="E4383">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4384" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4384" s="1">
+        <v>43558.872916666667</v>
+      </c>
+      <c r="D4384">
+        <v>0</v>
+      </c>
+      <c r="E4384">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4385" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4385" s="1">
+        <v>43558.883333333331</v>
+      </c>
+      <c r="D4385">
+        <v>0</v>
+      </c>
+      <c r="E4385">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4386" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4386" s="1">
+        <v>43558.893750000003</v>
+      </c>
+      <c r="D4386">
+        <v>0</v>
+      </c>
+      <c r="E4386">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4387" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4387" s="1">
+        <v>43558.904166666667</v>
+      </c>
+      <c r="D4387">
+        <v>0</v>
+      </c>
+      <c r="E4387">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4388" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4388" s="1">
+        <v>43558.919444444444</v>
+      </c>
+      <c r="D4388">
+        <v>1</v>
+      </c>
+      <c r="F4388">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4389" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4389" s="1">
+        <v>43558.928472222222</v>
+      </c>
+      <c r="D4389">
+        <v>0</v>
+      </c>
+      <c r="E4389">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4390" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4390" s="1">
+        <v>43558.938888888886</v>
+      </c>
+      <c r="D4390">
+        <v>0</v>
+      </c>
+      <c r="E4390">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4391" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4391" s="1">
+        <v>43558.949305555558</v>
+      </c>
+      <c r="D4391">
+        <v>0</v>
+      </c>
+      <c r="E4391">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4392" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4392" s="1">
+        <v>43558.959722222222</v>
+      </c>
+      <c r="D4392">
+        <v>0</v>
+      </c>
+      <c r="E4392">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4393" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4393" s="1">
+        <v>43558.970138888886</v>
+      </c>
+      <c r="D4393">
+        <v>0</v>
+      </c>
+      <c r="E4393">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4394" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4394" s="1">
+        <v>43558.980555555558</v>
+      </c>
+      <c r="D4394">
+        <v>0</v>
+      </c>
+      <c r="E4394">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4395" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4395" s="1">
+        <v>43558.990972222222</v>
+      </c>
+      <c r="D4395">
+        <v>0</v>
+      </c>
+      <c r="E4395">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4396" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4396" s="1">
+        <v>43559.001388888886</v>
+      </c>
+      <c r="D4396">
+        <v>0</v>
+      </c>
+      <c r="E4396">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4397" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4397" s="1">
+        <v>43559.011805555558</v>
+      </c>
+      <c r="D4397">
+        <v>0</v>
+      </c>
+      <c r="E4397">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4398" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4398" s="1">
+        <v>43559.022222222222</v>
+      </c>
+      <c r="D4398">
+        <v>0</v>
+      </c>
+      <c r="E4398">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4399" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4399" s="1">
+        <v>43559.032638888886</v>
+      </c>
+      <c r="D4399">
+        <v>0</v>
+      </c>
+      <c r="E4399">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4400" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4400" s="1">
+        <v>43559.043055555558</v>
+      </c>
+      <c r="D4400">
+        <v>0</v>
+      </c>
+      <c r="E4400">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4401" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4401" s="1">
+        <v>43559.053472222222</v>
+      </c>
+      <c r="D4401">
+        <v>0</v>
+      </c>
+      <c r="E4401">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4402" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4402" s="1">
+        <v>43559.063888888886</v>
+      </c>
+      <c r="D4402">
+        <v>0</v>
+      </c>
+      <c r="E4402">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4403" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4403" s="1">
+        <v>43559.074305555558</v>
+      </c>
+      <c r="D4403">
+        <v>0</v>
+      </c>
+      <c r="E4403">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4404" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4404" s="1">
+        <v>43559.084722222222</v>
+      </c>
+      <c r="D4404">
+        <v>0</v>
+      </c>
+      <c r="E4404">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4405" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4405" s="1">
+        <v>43559.095138888886</v>
+      </c>
+      <c r="D4405">
+        <v>0</v>
+      </c>
+      <c r="E4405">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4406" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4406" s="1">
+        <v>43559.105555555558</v>
+      </c>
+      <c r="D4406">
+        <v>0</v>
+      </c>
+      <c r="E4406">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4407" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4407" s="1">
+        <v>43559.115972222222</v>
+      </c>
+      <c r="D4407">
+        <v>0</v>
+      </c>
+      <c r="E4407">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4408" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4408" s="1">
+        <v>43559.126388888886</v>
+      </c>
+      <c r="D4408">
+        <v>0</v>
+      </c>
+      <c r="E4408">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4409" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4409" s="1">
+        <v>43559.136805555558</v>
+      </c>
+      <c r="D4409">
+        <v>0</v>
+      </c>
+      <c r="E4409">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4410" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4410" s="1">
+        <v>43559.147222222222</v>
+      </c>
+      <c r="D4410">
+        <v>0</v>
+      </c>
+      <c r="E4410">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4411" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4411" s="1">
+        <v>43559.157638888886</v>
+      </c>
+      <c r="D4411">
+        <v>0</v>
+      </c>
+      <c r="E4411">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4412" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4412" s="1">
+        <v>43559.168055555558</v>
+      </c>
+      <c r="D4412">
+        <v>0</v>
+      </c>
+      <c r="E4412">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4413" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4413" s="1">
+        <v>43559.178472222222</v>
+      </c>
+      <c r="D4413">
+        <v>0</v>
+      </c>
+      <c r="E4413">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4414" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4414" s="1">
+        <v>43559.188888888886</v>
+      </c>
+      <c r="D4414">
+        <v>0</v>
+      </c>
+      <c r="E4414">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4415" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4415" s="1">
+        <v>43559.199305555558</v>
+      </c>
+      <c r="D4415">
+        <v>0</v>
+      </c>
+      <c r="E4415">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4416" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4416" s="1">
+        <v>43559.209722222222</v>
+      </c>
+      <c r="D4416">
+        <v>0</v>
+      </c>
+      <c r="E4416">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4417" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4417" s="1">
+        <v>43559.220138888886</v>
+      </c>
+      <c r="D4417">
+        <v>0</v>
+      </c>
+      <c r="E4417">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4418" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4418" s="1">
+        <v>43559.230555555558</v>
+      </c>
+      <c r="D4418">
+        <v>0</v>
+      </c>
+      <c r="E4418">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4419" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4419" s="1">
+        <v>43559.240972222222</v>
+      </c>
+      <c r="D4419">
+        <v>0</v>
+      </c>
+      <c r="E4419">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4420" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4420" s="1">
+        <v>43559.251388888886</v>
+      </c>
+      <c r="D4420">
+        <v>0</v>
+      </c>
+      <c r="E4420">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4421" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4421" s="1">
+        <v>43559.261111111111</v>
+      </c>
+      <c r="D4421">
+        <v>1</v>
+      </c>
+      <c r="F4421">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4422" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4422" s="1">
+        <v>43559.261111111111</v>
+      </c>
+      <c r="D4422">
+        <v>1</v>
+      </c>
+      <c r="F4422" s="3">
+        <v>77</v>
+      </c>
+      <c r="N4422">
+        <v>83</v>
+      </c>
+      <c r="O4422">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4423" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4423" s="1">
+        <v>43559.261805555558</v>
+      </c>
+      <c r="D4423">
+        <v>0</v>
+      </c>
+      <c r="E4423">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4424" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4424" s="1">
+        <v>43559.272222222222</v>
+      </c>
+      <c r="D4424">
+        <v>0</v>
+      </c>
+      <c r="E4424">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4425" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4425" s="1">
+        <v>43559.273611111108</v>
+      </c>
+      <c r="D4425">
+        <v>1</v>
+      </c>
+      <c r="F4425">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4426" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4426" s="1">
+        <v>43559.273611111108</v>
+      </c>
+      <c r="D4426">
+        <v>6</v>
+      </c>
+      <c r="F4426" s="3">
+        <v>82</v>
+      </c>
+      <c r="N4426">
+        <v>90</v>
+      </c>
+      <c r="O4426">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4427" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4427" s="1">
+        <v>43559.283333333333</v>
+      </c>
+      <c r="D4427">
+        <v>0</v>
+      </c>
+      <c r="E4427">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4428" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4428" s="1">
+        <v>43559.287499999999</v>
+      </c>
+      <c r="D4428">
+        <v>1</v>
+      </c>
+      <c r="F4428">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4429" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4429" s="1">
+        <v>43559.287499999999</v>
+      </c>
+      <c r="D4429">
+        <v>1</v>
+      </c>
+      <c r="F4429" s="3">
+        <v>95</v>
+      </c>
+      <c r="N4429">
+        <v>88</v>
+      </c>
+      <c r="O4429">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4430" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4430" s="1">
+        <v>43559.301388888889</v>
+      </c>
+      <c r="D4430">
+        <v>1</v>
+      </c>
+      <c r="F4430">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4431" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4431" s="1">
+        <v>43559.301388888889</v>
+      </c>
+      <c r="D4431">
+        <v>1</v>
+      </c>
+      <c r="F4431" s="3">
+        <v>103</v>
+      </c>
+      <c r="N4431">
+        <v>86</v>
+      </c>
+      <c r="O4431">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4432" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4432" s="1">
+        <v>43559.304166666669</v>
+      </c>
+      <c r="D4432">
+        <v>0</v>
+      </c>
+      <c r="E4432">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4433" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4433" s="1">
+        <v>43559.314583333333</v>
+      </c>
+      <c r="D4433">
+        <v>1</v>
+      </c>
+      <c r="F4433">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4434" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4434" s="1">
+        <v>43559.314583333333</v>
+      </c>
+      <c r="D4434">
+        <v>6</v>
+      </c>
+      <c r="F4434" s="3">
+        <v>78</v>
+      </c>
+      <c r="N4434">
+        <v>85</v>
+      </c>
+      <c r="O4434">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4435" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4435" s="1">
+        <v>43559.314583333333</v>
+      </c>
+      <c r="D4435">
+        <v>0</v>
+      </c>
+      <c r="E4435">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4436" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4436" s="1">
+        <v>43559.324999999997</v>
+      </c>
+      <c r="D4436">
+        <v>0</v>
+      </c>
+      <c r="E4436">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4437" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4437" s="1">
+        <v>43559.335416666669</v>
+      </c>
+      <c r="D4437">
+        <v>0</v>
+      </c>
+      <c r="E4437">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4438" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4438" s="1">
+        <v>43559.338194444441</v>
+      </c>
+      <c r="D4438">
+        <v>1</v>
+      </c>
+      <c r="F4438">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4439" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4439" s="1">
+        <v>43559.34097222222</v>
+      </c>
+      <c r="D4439">
+        <v>1</v>
+      </c>
+      <c r="F4439">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4440" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4440" s="1">
+        <v>43559.34097222222</v>
+      </c>
+      <c r="D4440">
+        <v>6</v>
+      </c>
+      <c r="F4440" s="3">
+        <v>80</v>
+      </c>
+      <c r="N4440" t="s">
+        <v>70</v>
+      </c>
+      <c r="O4440">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4441" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4441" s="1">
+        <v>43559.34652777778</v>
+      </c>
+      <c r="D4441">
+        <v>0</v>
+      </c>
+      <c r="E4441">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4442" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4442" s="1">
+        <v>43559.347222222219</v>
+      </c>
+      <c r="D4442">
+        <v>1</v>
+      </c>
+      <c r="F4442">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4443" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4443" s="1">
+        <v>43559.355555555558</v>
+      </c>
+      <c r="D4443">
+        <v>1</v>
+      </c>
+      <c r="F4443">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4444" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4444" s="1">
+        <v>43559.355555555558</v>
+      </c>
+      <c r="D4444">
+        <v>6</v>
+      </c>
+      <c r="F4444" s="3">
+        <v>79</v>
+      </c>
+      <c r="N4444">
+        <v>85</v>
+      </c>
+      <c r="O4444">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4445" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4445" s="1">
+        <v>43559.356249999997</v>
+      </c>
+      <c r="D4445">
+        <v>0</v>
+      </c>
+      <c r="E4445">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4446" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4446" s="1">
+        <v>43559.365972222222</v>
+      </c>
+      <c r="D4446">
+        <v>1</v>
+      </c>
+      <c r="F4446">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4447" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4447" s="1">
+        <v>43559.365972222222</v>
+      </c>
+      <c r="D4447">
+        <v>6</v>
+      </c>
+      <c r="F4447" s="3">
+        <v>110</v>
+      </c>
+      <c r="N4447">
+        <v>135</v>
+      </c>
+      <c r="O4447">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4448" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4448" s="1">
+        <v>43559.366666666669</v>
+      </c>
+      <c r="D4448">
+        <v>0</v>
+      </c>
+      <c r="E4448">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4449" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4449" s="1">
+        <v>43559.37777777778</v>
+      </c>
+      <c r="D4449">
+        <v>0</v>
+      </c>
+      <c r="E4449">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4450" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4450" s="1">
+        <v>43559.37777777778</v>
+      </c>
+      <c r="D4450">
+        <v>1</v>
+      </c>
+      <c r="F4450">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4451" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4451" s="1">
+        <v>43559.37777777778</v>
+      </c>
+      <c r="D4451">
+        <v>6</v>
+      </c>
+      <c r="F4451" s="3">
+        <v>147</v>
+      </c>
+      <c r="N4451">
+        <v>136</v>
+      </c>
+      <c r="O4451">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4452" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4452" s="1">
+        <v>43559.384722222225</v>
+      </c>
+      <c r="D4452">
+        <v>1</v>
+      </c>
+      <c r="F4452">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4453" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4453" s="1">
+        <v>43559.386111111111</v>
+      </c>
+      <c r="D4453">
+        <v>1</v>
+      </c>
+      <c r="F4453">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4454" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4454" s="1">
+        <v>43559.386111111111</v>
+      </c>
+      <c r="D4454">
+        <v>6</v>
+      </c>
+      <c r="F4454" s="3">
+        <v>127</v>
+      </c>
+      <c r="N4454">
+        <v>97</v>
+      </c>
+      <c r="O4454">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4455" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4455" s="1">
+        <v>43559.396527777775</v>
+      </c>
+      <c r="D4455">
+        <v>1</v>
+      </c>
+      <c r="F4455">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4456" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4456" s="1">
+        <v>43559.397916666669</v>
+      </c>
+      <c r="D4456">
+        <v>1</v>
+      </c>
+      <c r="F4456">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4457" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4457" s="1">
+        <v>43559.397916666669</v>
+      </c>
+      <c r="D4457">
+        <v>6</v>
+      </c>
+      <c r="F4457" s="3">
+        <v>96</v>
+      </c>
+      <c r="N4457">
+        <v>96</v>
+      </c>
+      <c r="O4457">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4458" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4458" s="1">
+        <v>43559.398611111108</v>
+      </c>
+      <c r="D4458">
+        <v>0</v>
+      </c>
+      <c r="E4458">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4459" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4459" s="1">
+        <v>43559.408333333333</v>
+      </c>
+      <c r="D4459">
+        <v>1</v>
+      </c>
+      <c r="F4459">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4460" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4460" s="1">
+        <v>43559.408333333333</v>
+      </c>
+      <c r="D4460">
+        <v>6</v>
+      </c>
+      <c r="F4460" s="3">
+        <v>73</v>
+      </c>
+      <c r="N4460">
+        <v>79</v>
+      </c>
+      <c r="O4460">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4461" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4461" s="1">
+        <v>43559.40902777778</v>
+      </c>
+      <c r="D4461">
+        <v>0</v>
+      </c>
+      <c r="E4461">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4462" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4462" s="1">
+        <v>43559.409722222219</v>
+      </c>
+      <c r="D4462">
+        <v>1</v>
+      </c>
+      <c r="F4462">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4463" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4463" s="1">
+        <v>43559.418749999997</v>
+      </c>
+      <c r="D4463">
+        <v>1</v>
+      </c>
+      <c r="F4463">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4464" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4464" s="1">
+        <v>43559.418749999997</v>
+      </c>
+      <c r="D4464">
+        <v>6</v>
+      </c>
+      <c r="N4464" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4465" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4465" s="1">
+        <v>43559.419444444444</v>
+      </c>
+      <c r="D4465">
+        <v>1</v>
+      </c>
+      <c r="F4465">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4466" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4466" s="1">
+        <v>43559.419444444444</v>
+      </c>
+      <c r="D4466">
+        <v>6</v>
+      </c>
+      <c r="F4466" s="3">
+        <v>61</v>
+      </c>
+      <c r="N4466">
+        <v>73</v>
+      </c>
+      <c r="O4466">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4467" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4467" s="1">
+        <v>43559.422222222223</v>
+      </c>
+      <c r="D4467">
+        <v>0</v>
+      </c>
+      <c r="E4467">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4468" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4468" s="1">
+        <v>43559.432638888888</v>
+      </c>
+      <c r="D4468">
+        <v>0</v>
+      </c>
+      <c r="E4468">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4469" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4469" s="1">
+        <v>43559.443055555559</v>
+      </c>
+      <c r="D4469">
+        <v>0</v>
+      </c>
+      <c r="E4469">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4470" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4470" s="1">
+        <v>43559.453472222223</v>
+      </c>
+      <c r="D4470">
+        <v>0</v>
+      </c>
+      <c r="E4470">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4471" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4471" s="1">
+        <v>43559.463888888888</v>
+      </c>
+      <c r="D4471">
+        <v>0</v>
+      </c>
+      <c r="E4471">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4472" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4472" s="1">
+        <v>43559.474305555559</v>
+      </c>
+      <c r="D4472">
+        <v>0</v>
+      </c>
+      <c r="E4472">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4473" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4473" s="1">
+        <v>43559.484722222223</v>
+      </c>
+      <c r="D4473">
+        <v>0</v>
+      </c>
+      <c r="E4473">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4474" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4474" s="1">
+        <v>43559.495138888888</v>
+      </c>
+      <c r="D4474">
+        <v>0</v>
+      </c>
+      <c r="E4474">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4475" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4475" s="1">
+        <v>43559.505555555559</v>
+      </c>
+      <c r="D4475">
+        <v>0</v>
+      </c>
+      <c r="E4475">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4476" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4476" s="1">
+        <v>43559.515972222223</v>
+      </c>
+      <c r="D4476">
+        <v>0</v>
+      </c>
+      <c r="E4476">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4477" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4477" s="1">
+        <v>43559.526388888888</v>
+      </c>
+      <c r="D4477">
+        <v>0</v>
+      </c>
+      <c r="E4477">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4478" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4478" s="1">
+        <v>43559.536805555559</v>
+      </c>
+      <c r="D4478">
+        <v>0</v>
+      </c>
+      <c r="E4478">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4479" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4479" s="1">
+        <v>43559.547222222223</v>
+      </c>
+      <c r="D4479">
+        <v>0</v>
+      </c>
+      <c r="E4479">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4480" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4480" s="1">
+        <v>43559.557638888888</v>
+      </c>
+      <c r="D4480">
+        <v>0</v>
+      </c>
+      <c r="E4480">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4481" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4481" s="1">
+        <v>43559.568055555559</v>
+      </c>
+      <c r="D4481">
+        <v>0</v>
+      </c>
+      <c r="E4481">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4482" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4482" s="1">
+        <v>43559.578472222223</v>
+      </c>
+      <c r="D4482">
+        <v>0</v>
+      </c>
+      <c r="E4482">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4483" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4483" s="1">
+        <v>43559.588888888888</v>
+      </c>
+      <c r="D4483">
+        <v>0</v>
+      </c>
+      <c r="E4483">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4484" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4484" s="1">
+        <v>43559.599305555559</v>
+      </c>
+      <c r="D4484">
+        <v>0</v>
+      </c>
+      <c r="E4484">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4485" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4485" s="1">
+        <v>43559.609722222223</v>
+      </c>
+      <c r="D4485">
+        <v>0</v>
+      </c>
+      <c r="E4485">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4486" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4486" s="1">
+        <v>43559.620138888888</v>
+      </c>
+      <c r="D4486">
+        <v>0</v>
+      </c>
+      <c r="E4486">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4487" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4487" s="1">
+        <v>43559.630555555559</v>
+      </c>
+      <c r="D4487">
+        <v>0</v>
+      </c>
+      <c r="E4487">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4488" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4488" s="1">
+        <v>43559.640972222223</v>
+      </c>
+      <c r="D4488">
+        <v>0</v>
+      </c>
+      <c r="E4488">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4489" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4489" s="1">
+        <v>43559.651388888888</v>
+      </c>
+      <c r="D4489">
+        <v>0</v>
+      </c>
+      <c r="E4489">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4490" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4490" s="1">
+        <v>43559.661805555559</v>
+      </c>
+      <c r="D4490">
+        <v>0</v>
+      </c>
+      <c r="E4490">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4491" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4491" s="1">
+        <v>43559.672222222223</v>
+      </c>
+      <c r="D4491">
+        <v>0</v>
+      </c>
+      <c r="E4491">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4492" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4492" s="1">
+        <v>43559.682638888888</v>
+      </c>
+      <c r="D4492">
+        <v>0</v>
+      </c>
+      <c r="E4492">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4493" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4493" s="1">
+        <v>43559.693055555559</v>
+      </c>
+      <c r="D4493">
+        <v>0</v>
+      </c>
+      <c r="E4493">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4494" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4494" s="1">
+        <v>43559.703472222223</v>
+      </c>
+      <c r="D4494">
+        <v>0</v>
+      </c>
+      <c r="E4494">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4495" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4495" s="1">
+        <v>43559.713888888888</v>
+      </c>
+      <c r="D4495">
+        <v>0</v>
+      </c>
+      <c r="E4495">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4496" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4496" s="1">
+        <v>43559.724305555559</v>
+      </c>
+      <c r="D4496">
+        <v>0</v>
+      </c>
+      <c r="E4496">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4497" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4497" s="1">
+        <v>43559.743750000001</v>
+      </c>
+      <c r="D4497">
+        <v>1</v>
+      </c>
+      <c r="F4497">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4498" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4498" s="1">
+        <v>43559.746527777781</v>
+      </c>
+      <c r="D4498">
+        <v>0</v>
+      </c>
+      <c r="E4498">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4499" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4499" s="1">
+        <v>43559.756944444445</v>
+      </c>
+      <c r="D4499">
+        <v>0</v>
+      </c>
+      <c r="E4499">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4500" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4500" s="1">
+        <v>43559.767361111109</v>
+      </c>
+      <c r="D4500">
+        <v>0</v>
+      </c>
+      <c r="E4500">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4501" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4501" s="1">
+        <v>43559.777777777781</v>
+      </c>
+      <c r="D4501">
+        <v>0</v>
+      </c>
+      <c r="E4501">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4502" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4502" s="1">
+        <v>43559.788194444445</v>
+      </c>
+      <c r="D4502">
+        <v>0</v>
+      </c>
+      <c r="E4502">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4503" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4503" s="1">
+        <v>43559.798611111109</v>
+      </c>
+      <c r="D4503">
+        <v>0</v>
+      </c>
+      <c r="E4503">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4504" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4504" s="1">
+        <v>43559.809027777781</v>
+      </c>
+      <c r="D4504">
+        <v>0</v>
+      </c>
+      <c r="E4504">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4505" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4505" s="1">
+        <v>43559.819444444445</v>
+      </c>
+      <c r="D4505">
+        <v>0</v>
+      </c>
+      <c r="E4505">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4506" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4506" s="1">
+        <v>43559.829861111109</v>
+      </c>
+      <c r="D4506">
+        <v>0</v>
+      </c>
+      <c r="E4506">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4507" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4507" s="1">
+        <v>43559.841666666667</v>
+      </c>
+      <c r="D4507">
+        <v>0</v>
+      </c>
+      <c r="E4507">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4508" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4508" s="1">
+        <v>43559.848611111112</v>
+      </c>
+      <c r="D4508">
+        <v>1</v>
+      </c>
+      <c r="F4508">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4509" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4509" s="1">
+        <v>43559.852083333331</v>
+      </c>
+      <c r="D4509">
+        <v>0</v>
+      </c>
+      <c r="E4509">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4510" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4510" s="1">
+        <v>43559.862500000003</v>
+      </c>
+      <c r="D4510">
+        <v>0</v>
+      </c>
+      <c r="E4510">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4511" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4511" s="1">
+        <v>43559.872916666667</v>
+      </c>
+      <c r="D4511">
+        <v>0</v>
+      </c>
+      <c r="E4511">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4512" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4512" s="1">
+        <v>43559.883333333331</v>
+      </c>
+      <c r="D4512">
+        <v>0</v>
+      </c>
+      <c r="E4512">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4513" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4513" s="1">
+        <v>43559.893750000003</v>
+      </c>
+      <c r="D4513">
+        <v>0</v>
+      </c>
+      <c r="E4513">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4514" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4514" s="1">
+        <v>43559.904166666667</v>
+      </c>
+      <c r="D4514">
+        <v>0</v>
+      </c>
+      <c r="E4514">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4515" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4515" s="1">
+        <v>43559.914583333331</v>
+      </c>
+      <c r="D4515">
+        <v>0</v>
+      </c>
+      <c r="E4515">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4516" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4516" s="1">
+        <v>43559.925000000003</v>
+      </c>
+      <c r="D4516">
+        <v>1</v>
+      </c>
+      <c r="F4516">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4517" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4517" s="1">
+        <v>43559.927777777775</v>
+      </c>
+      <c r="D4517">
+        <v>0</v>
+      </c>
+      <c r="E4517">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4518" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4518" s="1">
+        <v>43559.938194444447</v>
+      </c>
+      <c r="D4518">
+        <v>0</v>
+      </c>
+      <c r="E4518">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4519" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4519" s="1">
+        <v>43559.948611111111</v>
+      </c>
+      <c r="D4519">
+        <v>0</v>
+      </c>
+      <c r="E4519">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4520" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4520" s="1">
+        <v>43559.959027777775</v>
+      </c>
+      <c r="D4520">
+        <v>0</v>
+      </c>
+      <c r="E4520">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4521" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4521" s="1">
+        <v>43559.969444444447</v>
+      </c>
+      <c r="D4521">
+        <v>0</v>
+      </c>
+      <c r="E4521">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4522" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4522" s="1">
+        <v>43559.979861111111</v>
+      </c>
+      <c r="D4522">
+        <v>0</v>
+      </c>
+      <c r="E4522">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4523" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4523" s="1">
+        <v>43559.990277777775</v>
+      </c>
+      <c r="D4523">
+        <v>0</v>
+      </c>
+      <c r="E4523">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4524" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4524" s="1">
+        <v>43560.000694444447</v>
+      </c>
+      <c r="D4524">
+        <v>0</v>
+      </c>
+      <c r="E4524">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4525" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4525" s="1">
+        <v>43560.011111111111</v>
+      </c>
+      <c r="D4525">
+        <v>0</v>
+      </c>
+      <c r="E4525">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4526" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4526" s="1">
+        <v>43560.021527777775</v>
+      </c>
+      <c r="D4526">
+        <v>0</v>
+      </c>
+      <c r="E4526">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4527" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4527" s="1">
+        <v>43560.031944444447</v>
+      </c>
+      <c r="D4527">
+        <v>0</v>
+      </c>
+      <c r="E4527">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4528" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4528" s="1">
+        <v>43560.042361111111</v>
+      </c>
+      <c r="D4528">
+        <v>0</v>
+      </c>
+      <c r="E4528">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4529" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4529" s="1">
+        <v>43560.052777777775</v>
+      </c>
+      <c r="D4529">
+        <v>0</v>
+      </c>
+      <c r="E4529">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4530" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4530" s="1">
+        <v>43560.063194444447</v>
+      </c>
+      <c r="D4530">
+        <v>0</v>
+      </c>
+      <c r="E4530">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4531" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4531" s="1">
+        <v>43560.073611111111</v>
+      </c>
+      <c r="D4531">
+        <v>0</v>
+      </c>
+      <c r="E4531">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4532" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4532" s="1">
+        <v>43560.084027777775</v>
+      </c>
+      <c r="D4532">
+        <v>0</v>
+      </c>
+      <c r="E4532">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4533" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4533" s="1">
+        <v>43560.094444444447</v>
+      </c>
+      <c r="D4533">
+        <v>0</v>
+      </c>
+      <c r="E4533">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4534" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4534" s="1">
+        <v>43560.104861111111</v>
+      </c>
+      <c r="D4534">
+        <v>0</v>
+      </c>
+      <c r="E4534">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4535" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4535" s="1">
+        <v>43560.115277777775</v>
+      </c>
+      <c r="D4535">
+        <v>0</v>
+      </c>
+      <c r="E4535">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4536" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4536" s="1">
+        <v>43560.125694444447</v>
+      </c>
+      <c r="D4536">
+        <v>0</v>
+      </c>
+      <c r="E4536">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4537" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4537" s="1">
+        <v>43560.136111111111</v>
+      </c>
+      <c r="D4537">
+        <v>0</v>
+      </c>
+      <c r="E4537">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4538" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4538" s="1">
+        <v>43560.146527777775</v>
+      </c>
+      <c r="D4538">
+        <v>0</v>
+      </c>
+      <c r="E4538">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4539" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4539" s="1">
+        <v>43560.156944444447</v>
+      </c>
+      <c r="D4539">
+        <v>0</v>
+      </c>
+      <c r="E4539">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4540" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4540" s="1">
+        <v>43560.167361111111</v>
+      </c>
+      <c r="D4540">
+        <v>0</v>
+      </c>
+      <c r="E4540">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4541" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4541" s="1">
+        <v>43560.177777777775</v>
+      </c>
+      <c r="D4541">
+        <v>0</v>
+      </c>
+      <c r="E4541">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4542" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4542" s="1">
+        <v>43560.188194444447</v>
+      </c>
+      <c r="D4542">
+        <v>0</v>
+      </c>
+      <c r="E4542">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4543" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4543" s="1">
+        <v>43560.198611111111</v>
+      </c>
+      <c r="D4543">
+        <v>0</v>
+      </c>
+      <c r="E4543">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4544" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4544" s="1">
+        <v>43560.209027777775</v>
+      </c>
+      <c r="D4544">
+        <v>0</v>
+      </c>
+      <c r="E4544">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4545" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4545" s="1">
+        <v>43560.219444444447</v>
+      </c>
+      <c r="D4545">
+        <v>0</v>
+      </c>
+      <c r="E4545">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4546" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4546" s="1">
+        <v>43560.230555555558</v>
+      </c>
+      <c r="D4546">
+        <v>0</v>
+      </c>
+      <c r="E4546">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4547" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4547" s="1">
+        <v>43560.239583333336</v>
+      </c>
+      <c r="D4547">
+        <v>1</v>
+      </c>
+      <c r="F4547">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4548" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4548" s="1">
+        <v>43560.240972222222</v>
+      </c>
+      <c r="D4548">
+        <v>0</v>
+      </c>
+      <c r="E4548">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4549" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4549" s="1">
+        <v>43560.251388888886</v>
+      </c>
+      <c r="D4549">
+        <v>0</v>
+      </c>
+      <c r="E4549">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4550" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4550" s="1">
+        <v>43560.261805555558</v>
+      </c>
+      <c r="D4550">
+        <v>0</v>
+      </c>
+      <c r="E4550">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4551" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4551" s="1">
+        <v>43560.272222222222</v>
+      </c>
+      <c r="D4551">
+        <v>0</v>
+      </c>
+      <c r="E4551">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4552" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4552" s="1">
+        <v>43560.282638888886</v>
+      </c>
+      <c r="D4552">
+        <v>0</v>
+      </c>
+      <c r="E4552">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4553" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4553" s="1">
+        <v>43560.293055555558</v>
+      </c>
+      <c r="D4553">
+        <v>0</v>
+      </c>
+      <c r="E4553">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4554" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4554" s="1">
+        <v>43560.303472222222</v>
+      </c>
+      <c r="D4554">
+        <v>0</v>
+      </c>
+      <c r="E4554">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4555" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4555" s="1">
+        <v>43560.313888888886</v>
+      </c>
+      <c r="D4555">
+        <v>0</v>
+      </c>
+      <c r="E4555">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4556" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4556" s="1">
+        <v>43560.324305555558</v>
+      </c>
+      <c r="D4556">
+        <v>0</v>
+      </c>
+      <c r="E4556">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4557" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4557" s="1">
+        <v>43560.334722222222</v>
+      </c>
+      <c r="D4557">
+        <v>0</v>
+      </c>
+      <c r="E4557">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4558" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4558" s="1">
+        <v>43560.341666666667</v>
+      </c>
+      <c r="D4558">
+        <v>1</v>
+      </c>
+      <c r="F4558">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4559" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4559" s="1">
+        <v>43560.345138888886</v>
+      </c>
+      <c r="D4559">
+        <v>0</v>
+      </c>
+      <c r="E4559">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4560" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4560" s="1">
+        <v>43560.356944444444</v>
+      </c>
+      <c r="D4560">
+        <v>0</v>
+      </c>
+      <c r="E4560">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4561" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4561" s="1">
+        <v>43560.359027777777</v>
+      </c>
+      <c r="D4561">
+        <v>1</v>
+      </c>
+      <c r="F4561">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4562" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4562" s="1">
+        <v>43560.359027777777</v>
+      </c>
+      <c r="D4562">
+        <v>6</v>
+      </c>
+      <c r="F4562" s="3">
+        <v>76</v>
+      </c>
+      <c r="N4562">
+        <v>82</v>
+      </c>
+      <c r="O4562" s="3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4563" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4563" s="1">
+        <v>43560.367361111108</v>
+      </c>
+      <c r="D4563">
+        <v>0</v>
+      </c>
+      <c r="E4563">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4564" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4564" s="1">
+        <v>43560.37777777778</v>
+      </c>
+      <c r="D4564">
+        <v>0</v>
+      </c>
+      <c r="E4564">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4565" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4565" s="1">
+        <v>43560.388194444444</v>
+      </c>
+      <c r="D4565">
+        <v>0</v>
+      </c>
+      <c r="E4565">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4566" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4566" s="1">
+        <v>43560.398611111108</v>
+      </c>
+      <c r="D4566">
+        <v>0</v>
+      </c>
+      <c r="E4566">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4567" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4567" s="1">
+        <v>43560.40902777778</v>
+      </c>
+      <c r="D4567">
+        <v>0</v>
+      </c>
+      <c r="E4567">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4568" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4568" s="1">
+        <v>43560.419444444444</v>
+      </c>
+      <c r="D4568">
+        <v>0</v>
+      </c>
+      <c r="E4568">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4569" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4569" s="1">
+        <v>43560.438888888886</v>
+      </c>
+      <c r="D4569">
+        <v>1</v>
+      </c>
+      <c r="F4569">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4570" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4570" s="1">
+        <v>43560.441666666666</v>
+      </c>
+      <c r="D4570">
+        <v>0</v>
+      </c>
+      <c r="E4570">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4571" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4571" s="1">
+        <v>43560.45208333333</v>
+      </c>
+      <c r="D4571">
+        <v>0</v>
+      </c>
+      <c r="E4571">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4572" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4572" s="1">
+        <v>43560.462500000001</v>
+      </c>
+      <c r="D4572">
+        <v>0</v>
+      </c>
+      <c r="E4572">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4573" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4573" s="1">
+        <v>43560.472916666666</v>
+      </c>
+      <c r="D4573">
+        <v>0</v>
+      </c>
+      <c r="E4573">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4574" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4574" s="1">
+        <v>43560.48333333333</v>
+      </c>
+      <c r="D4574">
+        <v>0</v>
+      </c>
+      <c r="E4574">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4575" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4575" s="1">
+        <v>43560.493750000001</v>
+      </c>
+      <c r="D4575">
+        <v>0</v>
+      </c>
+      <c r="E4575">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4576" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4576" s="1">
+        <v>43560.504166666666</v>
+      </c>
+      <c r="D4576">
+        <v>0</v>
+      </c>
+      <c r="E4576">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4577" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4577" s="1">
+        <v>43560.51458333333</v>
+      </c>
+      <c r="D4577">
+        <v>0</v>
+      </c>
+      <c r="E4577">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4578" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4578" s="1">
+        <v>43560.525000000001</v>
+      </c>
+      <c r="D4578">
+        <v>0</v>
+      </c>
+      <c r="E4578">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4579" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4579" s="1">
+        <v>43560.535416666666</v>
+      </c>
+      <c r="D4579">
+        <v>0</v>
+      </c>
+      <c r="E4579">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4580" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4580" s="1">
+        <v>43560.54583333333</v>
+      </c>
+      <c r="D4580">
+        <v>0</v>
+      </c>
+      <c r="E4580">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4581" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4581" s="1">
+        <v>43560.556250000001</v>
+      </c>
+      <c r="D4581">
+        <v>0</v>
+      </c>
+      <c r="E4581">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4582" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4582" s="1">
+        <v>43560.566666666666</v>
+      </c>
+      <c r="D4582">
+        <v>0</v>
+      </c>
+      <c r="E4582">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4583" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4583" s="1">
+        <v>43560.57708333333</v>
+      </c>
+      <c r="D4583">
+        <v>0</v>
+      </c>
+      <c r="E4583">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4584" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4584" s="1">
+        <v>43560.587500000001</v>
+      </c>
+      <c r="D4584">
+        <v>0</v>
+      </c>
+      <c r="E4584">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4585" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4585" s="1">
+        <v>43560.597916666666</v>
+      </c>
+      <c r="D4585">
+        <v>0</v>
+      </c>
+      <c r="E4585">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4586" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4586" s="1">
+        <v>43560.61041666667</v>
+      </c>
+      <c r="D4586">
+        <v>0</v>
+      </c>
+      <c r="E4586">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4587" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4587" s="1">
+        <v>43560.615972222222</v>
+      </c>
+      <c r="D4587">
+        <v>1</v>
+      </c>
+      <c r="F4587">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4588" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4588" s="1">
+        <v>43560.620833333334</v>
+      </c>
+      <c r="D4588">
+        <v>0</v>
+      </c>
+      <c r="E4588">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4589" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4589" s="1">
+        <v>43560.631249999999</v>
+      </c>
+      <c r="D4589">
+        <v>0</v>
+      </c>
+      <c r="E4589">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4590" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4590" s="1">
+        <v>43560.64166666667</v>
+      </c>
+      <c r="D4590">
+        <v>0</v>
+      </c>
+      <c r="E4590">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4591" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4591" s="1">
+        <v>43560.652083333334</v>
+      </c>
+      <c r="D4591">
+        <v>0</v>
+      </c>
+      <c r="E4591">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4592" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4592" s="1">
+        <v>43560.662499999999</v>
+      </c>
+      <c r="D4592">
+        <v>0</v>
+      </c>
+      <c r="E4592">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4593" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4593" s="1">
+        <v>43560.67291666667</v>
+      </c>
+      <c r="D4593">
+        <v>0</v>
+      </c>
+      <c r="E4593">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4594" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4594" s="1">
+        <v>43560.683333333334</v>
+      </c>
+      <c r="D4594">
+        <v>0</v>
+      </c>
+      <c r="E4594">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4595" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4595" s="1">
+        <v>43560.693749999999</v>
+      </c>
+      <c r="D4595">
+        <v>0</v>
+      </c>
+      <c r="E4595">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4596" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4596" s="1">
+        <v>43560.70416666667</v>
+      </c>
+      <c r="D4596">
+        <v>0</v>
+      </c>
+      <c r="E4596">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4597" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4597" s="1">
+        <v>43560.714583333334</v>
+      </c>
+      <c r="D4597">
+        <v>0</v>
+      </c>
+      <c r="E4597">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4598" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4598" s="1">
+        <v>43560.724999999999</v>
+      </c>
+      <c r="D4598">
+        <v>0</v>
+      </c>
+      <c r="E4598">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4599" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4599" s="1">
+        <v>43560.73541666667</v>
+      </c>
+      <c r="D4599">
+        <v>0</v>
+      </c>
+      <c r="E4599">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4600" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4600" s="1">
+        <v>43560.745833333334</v>
+      </c>
+      <c r="D4600">
+        <v>0</v>
+      </c>
+      <c r="E4600">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4601" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4601" s="1">
+        <v>43560.756249999999</v>
+      </c>
+      <c r="D4601">
+        <v>0</v>
+      </c>
+      <c r="E4601">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4602" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4602" s="1">
+        <v>43560.76666666667</v>
+      </c>
+      <c r="D4602">
+        <v>0</v>
+      </c>
+      <c r="E4602">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4603" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4603" s="1">
+        <v>43560.777083333334</v>
+      </c>
+      <c r="D4603">
+        <v>0</v>
+      </c>
+      <c r="E4603">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4604" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4604" s="1">
+        <v>43560.787499999999</v>
+      </c>
+      <c r="D4604">
+        <v>0</v>
+      </c>
+      <c r="E4604">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4605" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4605" s="1">
+        <v>43560.79791666667</v>
+      </c>
+      <c r="D4605">
+        <v>0</v>
+      </c>
+      <c r="E4605">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4606" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4606" s="1">
+        <v>43560.809027777781</v>
+      </c>
+      <c r="D4606">
+        <v>0</v>
+      </c>
+      <c r="E4606">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4607" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4607" s="1">
+        <v>43560.80972222222</v>
+      </c>
+      <c r="D4607">
+        <v>1</v>
+      </c>
+      <c r="F4607">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4608" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4608" s="1">
+        <v>43560.819444444445</v>
+      </c>
+      <c r="D4608">
+        <v>0</v>
+      </c>
+      <c r="E4608">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4609" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4609" s="1">
+        <v>43560.829861111109</v>
+      </c>
+      <c r="D4609">
+        <v>0</v>
+      </c>
+      <c r="E4609">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4610" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4610" s="1">
+        <v>43560.840277777781</v>
+      </c>
+      <c r="D4610">
+        <v>0</v>
+      </c>
+      <c r="E4610">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4611" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4611" s="1">
+        <v>43560.850694444445</v>
+      </c>
+      <c r="D4611">
+        <v>0</v>
+      </c>
+      <c r="E4611">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4612" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4612" s="1">
+        <v>43560.861111111109</v>
+      </c>
+      <c r="D4612">
+        <v>0</v>
+      </c>
+      <c r="E4612">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4613" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4613" s="1">
+        <v>43560.873611111114</v>
+      </c>
+      <c r="D4613">
+        <v>0</v>
+      </c>
+      <c r="E4613">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4614" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4614" s="1">
+        <v>43560.875694444447</v>
+      </c>
+      <c r="D4614">
+        <v>1</v>
+      </c>
+      <c r="F4614">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4615" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4615" s="1">
+        <v>43560.884027777778</v>
+      </c>
+      <c r="D4615">
+        <v>0</v>
+      </c>
+      <c r="E4615">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4616" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4616" s="1">
+        <v>43560.894444444442</v>
+      </c>
+      <c r="D4616">
+        <v>0</v>
+      </c>
+      <c r="E4616">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4617" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4617" s="1">
+        <v>43560.904861111114</v>
+      </c>
+      <c r="D4617">
+        <v>0</v>
+      </c>
+      <c r="E4617">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4618" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4618" s="1">
+        <v>43560.915277777778</v>
+      </c>
+      <c r="D4618">
+        <v>0</v>
+      </c>
+      <c r="E4618">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4619" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4619" s="1">
+        <v>43560.925694444442</v>
+      </c>
+      <c r="D4619">
+        <v>0</v>
+      </c>
+      <c r="E4619">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4620" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4620" s="1">
+        <v>43560.936111111114</v>
+      </c>
+      <c r="D4620">
+        <v>0</v>
+      </c>
+      <c r="E4620">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4621" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4621" s="1">
+        <v>43560.946527777778</v>
+      </c>
+      <c r="D4621">
+        <v>0</v>
+      </c>
+      <c r="E4621">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4622" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4622" s="1">
+        <v>43560.956944444442</v>
+      </c>
+      <c r="D4622">
+        <v>0</v>
+      </c>
+      <c r="E4622">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4623" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4623" s="1">
+        <v>43560.967361111114</v>
+      </c>
+      <c r="D4623">
+        <v>0</v>
+      </c>
+      <c r="E4623">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4624" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4624" s="1">
+        <v>43560.977777777778</v>
+      </c>
+      <c r="D4624">
+        <v>0</v>
+      </c>
+      <c r="E4624">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4625" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4625" s="1">
+        <v>43560.988194444442</v>
+      </c>
+      <c r="D4625">
+        <v>0</v>
+      </c>
+      <c r="E4625">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4626" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4626" s="1">
+        <v>43560.998611111114</v>
+      </c>
+      <c r="D4626">
+        <v>0</v>
+      </c>
+      <c r="E4626">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4627" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4627" s="1">
+        <v>43561.009027777778</v>
+      </c>
+      <c r="D4627">
+        <v>0</v>
+      </c>
+      <c r="E4627">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4628" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4628" s="1">
+        <v>43561.019444444442</v>
+      </c>
+      <c r="D4628">
+        <v>0</v>
+      </c>
+      <c r="E4628">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4629" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4629" s="1">
+        <v>43561.029861111114</v>
+      </c>
+      <c r="D4629">
+        <v>0</v>
+      </c>
+      <c r="E4629">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4630" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4630" s="1">
+        <v>43561.040277777778</v>
+      </c>
+      <c r="D4630">
+        <v>0</v>
+      </c>
+      <c r="E4630">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4631" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4631" s="1">
+        <v>43561.050694444442</v>
+      </c>
+      <c r="D4631">
+        <v>0</v>
+      </c>
+      <c r="E4631">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4632" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4632" s="1">
+        <v>43561.061111111114</v>
+      </c>
+      <c r="D4632">
+        <v>0</v>
+      </c>
+      <c r="E4632">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4633" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4633" s="1">
+        <v>43561.071527777778</v>
+      </c>
+      <c r="D4633">
+        <v>0</v>
+      </c>
+      <c r="E4633">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4634" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4634" s="1">
+        <v>43561.083333333336</v>
+      </c>
+      <c r="D4634">
+        <v>0</v>
+      </c>
+      <c r="E4634">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4635" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4635" s="1">
+        <v>43561.087500000001</v>
+      </c>
+      <c r="D4635">
+        <v>1</v>
+      </c>
+      <c r="F4635">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4636" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4636" s="1">
+        <v>43561.09375</v>
+      </c>
+      <c r="D4636">
+        <v>0</v>
+      </c>
+      <c r="E4636">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4637" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4637" s="1">
+        <v>43561.104166666664</v>
+      </c>
+      <c r="D4637">
+        <v>0</v>
+      </c>
+      <c r="E4637">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4638" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4638" s="1">
+        <v>43561.114583333336</v>
+      </c>
+      <c r="D4638">
+        <v>0</v>
+      </c>
+      <c r="E4638">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4639" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4639" s="1">
+        <v>43561.125</v>
+      </c>
+      <c r="D4639">
+        <v>0</v>
+      </c>
+      <c r="E4639">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4640" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4640" s="1">
+        <v>43561.135416666664</v>
+      </c>
+      <c r="D4640">
+        <v>0</v>
+      </c>
+      <c r="E4640">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4641" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4641" s="1">
+        <v>43561.145833333336</v>
+      </c>
+      <c r="D4641">
+        <v>0</v>
+      </c>
+      <c r="E4641">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4642" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4642" s="1">
+        <v>43561.15625</v>
+      </c>
+      <c r="D4642">
+        <v>0</v>
+      </c>
+      <c r="E4642">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4643" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4643" s="1">
+        <v>43561.166666666664</v>
+      </c>
+      <c r="D4643">
+        <v>0</v>
+      </c>
+      <c r="E4643">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4644" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4644" s="1">
+        <v>43561.177083333336</v>
+      </c>
+      <c r="D4644">
+        <v>0</v>
+      </c>
+      <c r="E4644">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4645" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4645" s="1">
+        <v>43561.1875</v>
+      </c>
+      <c r="D4645">
+        <v>0</v>
+      </c>
+      <c r="E4645">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4646" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4646" s="1">
+        <v>43561.197916666664</v>
+      </c>
+      <c r="D4646">
+        <v>0</v>
+      </c>
+      <c r="E4646">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4647" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4647" s="1">
+        <v>43561.208333333336</v>
+      </c>
+      <c r="D4647">
+        <v>0</v>
+      </c>
+      <c r="E4647">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4648" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4648" s="1">
+        <v>43561.21875</v>
+      </c>
+      <c r="D4648">
+        <v>0</v>
+      </c>
+      <c r="E4648">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4649" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4649" s="1">
+        <v>43561.229166666664</v>
+      </c>
+      <c r="D4649">
+        <v>0</v>
+      </c>
+      <c r="E4649">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4650" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4650" s="1">
+        <v>43561.239583333336</v>
+      </c>
+      <c r="D4650">
+        <v>0</v>
+      </c>
+      <c r="E4650">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4651" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4651" s="1">
+        <v>43561.25</v>
+      </c>
+      <c r="D4651">
+        <v>0</v>
+      </c>
+      <c r="E4651">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4652" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4652" s="1">
+        <v>43561.260416666664</v>
+      </c>
+      <c r="D4652">
+        <v>0</v>
+      </c>
+      <c r="E4652">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4653" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4653" s="1">
+        <v>43561.271527777775</v>
+      </c>
+      <c r="D4653">
+        <v>0</v>
+      </c>
+      <c r="E4653">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4654" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4654" s="1">
+        <v>43561.277083333334</v>
+      </c>
+      <c r="D4654">
+        <v>1</v>
+      </c>
+      <c r="F4654">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4655" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4655" s="1">
+        <v>43561.27847222222</v>
+      </c>
+      <c r="D4655">
+        <v>1</v>
+      </c>
+      <c r="F4655">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4656" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C4656" s="1">
+        <v>43561.27847222222</v>
+      </c>
+      <c r="D4656">
+        <v>6</v>
+      </c>
+      <c r="F4656" s="3">
+        <v>84</v>
+      </c>
+      <c r="N4656">
+        <v>90</v>
+      </c>
+      <c r="O4656" s="3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4657" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4657" s="1">
+        <v>43561.281944444447</v>
+      </c>
+      <c r="D4657">
+        <v>0</v>
+      </c>
+      <c r="E4657">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4658" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4658" s="1">
+        <v>43561.292361111111</v>
+      </c>
+      <c r="D4658">
+        <v>0</v>
+      </c>
+      <c r="E4658">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4659" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4659" s="1">
+        <v>43561.302777777775</v>
+      </c>
+      <c r="D4659">
+        <v>0</v>
+      </c>
+      <c r="E4659">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4660" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4660" s="1">
+        <v>43561.314583333333</v>
+      </c>
+      <c r="D4660">
+        <v>1</v>
+      </c>
+      <c r="F4660">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4661" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4661" s="1">
+        <v>43561.314583333333</v>
+      </c>
+      <c r="D4661">
+        <v>0</v>
+      </c>
+      <c r="E4661">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4662" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4662" s="1">
+        <v>43561.324999999997</v>
+      </c>
+      <c r="D4662">
+        <v>0</v>
+      </c>
+      <c r="E4662">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4663" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4663" s="1">
+        <v>43561.335416666669</v>
+      </c>
+      <c r="D4663">
+        <v>0</v>
+      </c>
+      <c r="E4663">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4664" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4664" s="1">
+        <v>43561.345833333333</v>
+      </c>
+      <c r="D4664">
+        <v>0</v>
+      </c>
+      <c r="E4664">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4665" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4665" s="1">
+        <v>43561.356249999997</v>
+      </c>
+      <c r="D4665">
+        <v>0</v>
+      </c>
+      <c r="E4665">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4666" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4666" s="1">
+        <v>43561.366666666669</v>
+      </c>
+      <c r="D4666">
+        <v>0</v>
+      </c>
+      <c r="E4666">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4667" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4667" s="1">
+        <v>43561.377083333333</v>
+      </c>
+      <c r="D4667">
+        <v>0</v>
+      </c>
+      <c r="E4667">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4668" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4668" s="1">
+        <v>43561.387499999997</v>
+      </c>
+      <c r="D4668">
+        <v>0</v>
+      </c>
+      <c r="E4668">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4669" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4669" s="1">
+        <v>43561.397916666669</v>
+      </c>
+      <c r="D4669">
+        <v>0</v>
+      </c>
+      <c r="E4669">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4670" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4670" s="1">
+        <v>43561.408333333333</v>
+      </c>
+      <c r="D4670">
+        <v>0</v>
+      </c>
+      <c r="E4670">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4671" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4671" s="1">
+        <v>43561.418749999997</v>
+      </c>
+      <c r="D4671">
+        <v>0</v>
+      </c>
+      <c r="E4671">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4672" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4672" s="1">
+        <v>43561.429166666669</v>
+      </c>
+      <c r="D4672">
+        <v>0</v>
+      </c>
+      <c r="E4672">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4673" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C4673" s="1">
+        <v>43561.439583333333</v>
+      </c>
+      <c r="D4673">
+        <v>0</v>
+      </c>
+      <c r="E4673">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4674" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C4674" s="1">
+        <v>43561.45</v>
+      </c>
+      <c r="D4674">
+        <v>0</v>
+      </c>
+      <c r="E4674">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4675" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C4675" s="1">
+        <v>43561.460416666669</v>
+      </c>
+      <c r="D4675">
+        <v>0</v>
+      </c>
+      <c r="E4675">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4676" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C4676" s="1">
+        <v>43561.475694444445</v>
+      </c>
+      <c r="D4676">
+        <v>1</v>
+      </c>
+      <c r="F4676">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4677" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C4677" s="1">
+        <v>43561.477083333331</v>
+      </c>
+      <c r="D4677">
+        <v>1</v>
+      </c>
+      <c r="F4677">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4678" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C4678" s="1">
+        <v>43561.477083333331</v>
+      </c>
+      <c r="D4678">
+        <v>6</v>
+      </c>
+      <c r="F4678" s="3">
+        <v>80</v>
+      </c>
+      <c r="N4678">
+        <v>74</v>
+      </c>
+      <c r="P4678" s="3">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>